<commit_message>
Adding CAN message layout and signal descriptions
</commit_message>
<xml_diff>
--- a/1_Planning/System_Interface_Design.xlsx
+++ b/1_Planning/System_Interface_Design.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Signal List" sheetId="1" r:id="rId1"/>
+    <sheet name="CAN Messages" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="96">
   <si>
     <t>System Interface Design</t>
   </si>
@@ -237,13 +238,88 @@
   </si>
   <si>
     <t>paddle_velocity_cmd_mmps_y</t>
+  </si>
+  <si>
+    <t>CAN Message Layout</t>
+  </si>
+  <si>
+    <t>Message Name</t>
+  </si>
+  <si>
+    <t>Message ID (Hex)</t>
+  </si>
+  <si>
+    <t>DLC</t>
+  </si>
+  <si>
+    <t>Byte 3</t>
+  </si>
+  <si>
+    <t>Byte 2</t>
+  </si>
+  <si>
+    <t>Byte 1</t>
+  </si>
+  <si>
+    <t>Byte 0</t>
+  </si>
+  <si>
+    <t>0x100</t>
+  </si>
+  <si>
+    <t>0x101</t>
+  </si>
+  <si>
+    <t>Receiver</t>
+  </si>
+  <si>
+    <t>MC_Cmd_PC</t>
+  </si>
+  <si>
+    <t>PC_Status</t>
+  </si>
+  <si>
+    <t>pos_cmd_x_mm</t>
+  </si>
+  <si>
+    <t>pos_cmd_y_mm</t>
+  </si>
+  <si>
+    <t>pos_x_mm</t>
+  </si>
+  <si>
+    <t>pos_y_mm</t>
+  </si>
+  <si>
+    <t>CAN Signal Descriptions</t>
+  </si>
+  <si>
+    <t>Signal Name</t>
+  </si>
+  <si>
+    <t>Scaling Factor</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Initial Value</t>
+  </si>
+  <si>
+    <t>Length (Bits)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,6 +342,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -275,7 +357,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -283,15 +365,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,9 +729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1692,4 +1845,437 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AT6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" customWidth="1"/>
+    <col min="6" max="37" width="3.7109375" customWidth="1"/>
+    <col min="40" max="40" width="15.85546875" customWidth="1"/>
+    <col min="41" max="41" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="6" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:46" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="7"/>
+      <c r="AK2" s="7"/>
+      <c r="AN2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="AO2" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="AP2" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ2" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR2" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT2" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="8">
+        <v>7</v>
+      </c>
+      <c r="G3" s="8">
+        <v>6</v>
+      </c>
+      <c r="H3" s="8">
+        <v>5</v>
+      </c>
+      <c r="I3" s="8">
+        <v>4</v>
+      </c>
+      <c r="J3" s="8">
+        <v>3</v>
+      </c>
+      <c r="K3" s="8">
+        <v>2</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1</v>
+      </c>
+      <c r="M3" s="8">
+        <v>0</v>
+      </c>
+      <c r="N3" s="8">
+        <v>7</v>
+      </c>
+      <c r="O3" s="8">
+        <v>6</v>
+      </c>
+      <c r="P3" s="8">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>4</v>
+      </c>
+      <c r="R3" s="8">
+        <v>3</v>
+      </c>
+      <c r="S3" s="8">
+        <v>2</v>
+      </c>
+      <c r="T3" s="8">
+        <v>1</v>
+      </c>
+      <c r="U3" s="8">
+        <v>0</v>
+      </c>
+      <c r="V3" s="8">
+        <v>7</v>
+      </c>
+      <c r="W3" s="8">
+        <v>6</v>
+      </c>
+      <c r="X3" s="8">
+        <v>5</v>
+      </c>
+      <c r="Y3" s="8">
+        <v>4</v>
+      </c>
+      <c r="Z3" s="8">
+        <v>3</v>
+      </c>
+      <c r="AA3" s="8">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="8">
+        <v>7</v>
+      </c>
+      <c r="AE3" s="8">
+        <v>6</v>
+      </c>
+      <c r="AF3" s="8">
+        <v>5</v>
+      </c>
+      <c r="AG3" s="8">
+        <v>4</v>
+      </c>
+      <c r="AH3" s="8">
+        <v>3</v>
+      </c>
+      <c r="AI3" s="8">
+        <v>2</v>
+      </c>
+      <c r="AJ3" s="8">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO3" s="5">
+        <v>16</v>
+      </c>
+      <c r="AP3" s="12">
+        <v>1</v>
+      </c>
+      <c r="AQ3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="5">
+        <f>0+AQ3</f>
+        <v>0</v>
+      </c>
+      <c r="AS3" s="5">
+        <f>((2^AO3)*AP3)+AQ3</f>
+        <v>65536</v>
+      </c>
+      <c r="AT3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="5">
+        <v>4</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="10"/>
+      <c r="AH4" s="10"/>
+      <c r="AI4" s="10"/>
+      <c r="AJ4" s="10"/>
+      <c r="AK4" s="11"/>
+      <c r="AN4" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO4" s="5">
+        <v>16</v>
+      </c>
+      <c r="AP4" s="12">
+        <v>1</v>
+      </c>
+      <c r="AQ4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="5">
+        <f t="shared" ref="AR4:AR6" si="0">0+AQ4</f>
+        <v>0</v>
+      </c>
+      <c r="AS4" s="5">
+        <f t="shared" ref="AS4:AS6" si="1">((2^AO4)*AP4)+AQ4</f>
+        <v>65536</v>
+      </c>
+      <c r="AT4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="10"/>
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="10"/>
+      <c r="AK5" s="11"/>
+      <c r="AN5" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO5" s="5">
+        <v>16</v>
+      </c>
+      <c r="AP5" s="12">
+        <v>1</v>
+      </c>
+      <c r="AQ5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AS5" s="5">
+        <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="AT5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN6" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AO6" s="5">
+        <v>16</v>
+      </c>
+      <c r="AP6" s="12">
+        <v>1</v>
+      </c>
+      <c r="AQ6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AS6" s="5">
+        <f t="shared" si="1"/>
+        <v>65536</v>
+      </c>
+      <c r="AT6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="N2:U2"/>
+    <mergeCell ref="V2:AC2"/>
+    <mergeCell ref="AD2:AK2"/>
+    <mergeCell ref="F4:U4"/>
+    <mergeCell ref="V4:AK4"/>
+    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="V5:AK5"/>
+    <mergeCell ref="F5:U5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated CAN message layouts
</commit_message>
<xml_diff>
--- a/1_Planning/System_Interface_Design.xlsx
+++ b/1_Planning/System_Interface_Design.xlsx
@@ -1852,7 +1852,7 @@
   <dimension ref="A1:AT6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,7 +2099,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
@@ -2117,7 +2117,7 @@
       <c r="T4" s="10"/>
       <c r="U4" s="11"/>
       <c r="V4" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="W4" s="10"/>
       <c r="X4" s="10"/>
@@ -2175,7 +2175,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -2193,7 +2193,7 @@
       <c r="T5" s="10"/>
       <c r="U5" s="11"/>
       <c r="V5" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W5" s="10"/>
       <c r="X5" s="10"/>

</xml_diff>

<commit_message>
Adding separate messages for X and Y axis
</commit_message>
<xml_diff>
--- a/1_Planning/System_Interface_Design.xlsx
+++ b/1_Planning/System_Interface_Design.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="100">
   <si>
     <t>System Interface Design</t>
   </si>
@@ -276,9 +276,6 @@
     <t>MC_Cmd_PC</t>
   </si>
   <si>
-    <t>PC_Status</t>
-  </si>
-  <si>
     <t>pos_cmd_x_mm</t>
   </si>
   <si>
@@ -313,6 +310,21 @@
   </si>
   <si>
     <t>Length (Bits)</t>
+  </si>
+  <si>
+    <t>PC_Status_X</t>
+  </si>
+  <si>
+    <t>PC_Status_Y</t>
+  </si>
+  <si>
+    <t>PC_Y</t>
+  </si>
+  <si>
+    <t>PC_X</t>
+  </si>
+  <si>
+    <t>0x102</t>
   </si>
 </sst>
 </file>
@@ -357,7 +369,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -380,73 +392,30 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1852,7 +1821,7 @@
   <dimension ref="A1:AT6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1875,231 +1844,231 @@
         <v>71</v>
       </c>
       <c r="AN1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AN2" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="AO2" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AP2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AQ2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR2" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AS2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AT2" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="5">
+        <v>7</v>
+      </c>
+      <c r="G3" s="5">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5">
+        <v>5</v>
+      </c>
+      <c r="I3" s="5">
+        <v>4</v>
+      </c>
+      <c r="J3" s="5">
+        <v>3</v>
+      </c>
+      <c r="K3" s="5">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="7"/>
-      <c r="AA2" s="7"/>
-      <c r="AB2" s="7"/>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="7"/>
-      <c r="AN2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="AO2" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="AP2" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ2" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="AR2" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="AS2" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="AT2" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="8">
+      <c r="L3" s="5">
+        <v>1</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
         <v>7</v>
       </c>
-      <c r="G3" s="8">
+      <c r="O3" s="5">
         <v>6</v>
       </c>
-      <c r="H3" s="8">
+      <c r="P3" s="5">
         <v>5</v>
       </c>
-      <c r="I3" s="8">
+      <c r="Q3" s="5">
         <v>4</v>
       </c>
-      <c r="J3" s="8">
+      <c r="R3" s="5">
         <v>3</v>
       </c>
-      <c r="K3" s="8">
+      <c r="S3" s="5">
         <v>2</v>
       </c>
-      <c r="L3" s="8">
+      <c r="T3" s="5">
         <v>1</v>
       </c>
-      <c r="M3" s="8">
+      <c r="U3" s="5">
         <v>0</v>
       </c>
-      <c r="N3" s="8">
+      <c r="V3" s="5">
         <v>7</v>
       </c>
-      <c r="O3" s="8">
+      <c r="W3" s="5">
         <v>6</v>
       </c>
-      <c r="P3" s="8">
+      <c r="X3" s="5">
         <v>5</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="Y3" s="5">
         <v>4</v>
       </c>
-      <c r="R3" s="8">
+      <c r="Z3" s="5">
         <v>3</v>
       </c>
-      <c r="S3" s="8">
+      <c r="AA3" s="5">
         <v>2</v>
       </c>
-      <c r="T3" s="8">
+      <c r="AB3" s="5">
         <v>1</v>
       </c>
-      <c r="U3" s="8">
+      <c r="AC3" s="5">
         <v>0</v>
       </c>
-      <c r="V3" s="8">
+      <c r="AD3" s="5">
         <v>7</v>
       </c>
-      <c r="W3" s="8">
+      <c r="AE3" s="5">
         <v>6</v>
       </c>
-      <c r="X3" s="8">
+      <c r="AF3" s="5">
         <v>5</v>
       </c>
-      <c r="Y3" s="8">
+      <c r="AG3" s="5">
         <v>4</v>
       </c>
-      <c r="Z3" s="8">
+      <c r="AH3" s="5">
         <v>3</v>
       </c>
-      <c r="AA3" s="8">
+      <c r="AI3" s="5">
         <v>2</v>
       </c>
-      <c r="AB3" s="8">
+      <c r="AJ3" s="5">
         <v>1</v>
       </c>
-      <c r="AC3" s="8">
+      <c r="AK3" s="5">
         <v>0</v>
       </c>
-      <c r="AD3" s="8">
-        <v>7</v>
-      </c>
-      <c r="AE3" s="8">
-        <v>6</v>
-      </c>
-      <c r="AF3" s="8">
-        <v>5</v>
-      </c>
-      <c r="AG3" s="8">
-        <v>4</v>
-      </c>
-      <c r="AH3" s="8">
-        <v>3</v>
-      </c>
-      <c r="AI3" s="8">
-        <v>2</v>
-      </c>
-      <c r="AJ3" s="8">
+      <c r="AN3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO3" s="4">
+        <v>16</v>
+      </c>
+      <c r="AP3" s="6">
         <v>1</v>
       </c>
-      <c r="AK3" s="8">
+      <c r="AQ3" s="4">
         <v>0</v>
       </c>
-      <c r="AN3" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="AO3" s="5">
-        <v>16</v>
-      </c>
-      <c r="AP3" s="12">
-        <v>1</v>
-      </c>
-      <c r="AQ3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="5">
+      <c r="AR3" s="4">
         <f>0+AQ3</f>
         <v>0</v>
       </c>
-      <c r="AS3" s="5">
+      <c r="AS3" s="4">
         <f>((2^AO3)*AP3)+AQ3</f>
         <v>65536</v>
       </c>
-      <c r="AT3" s="5">
+      <c r="AT3" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>4</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>85</v>
+      <c r="F4" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
@@ -2115,9 +2084,9 @@
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="9" t="s">
-        <v>84</v>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="W4" s="10"/>
       <c r="X4" s="10"/>
@@ -2133,50 +2102,48 @@
       <c r="AH4" s="10"/>
       <c r="AI4" s="10"/>
       <c r="AJ4" s="10"/>
-      <c r="AK4" s="11"/>
-      <c r="AN4" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="AO4" s="5">
-        <v>16</v>
-      </c>
-      <c r="AP4" s="12">
+      <c r="AK4" s="10"/>
+      <c r="AN4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO4" s="4">
+        <v>16</v>
+      </c>
+      <c r="AP4" s="6">
         <v>1</v>
       </c>
-      <c r="AQ4" s="5">
+      <c r="AQ4" s="4">
         <v>0</v>
       </c>
-      <c r="AR4" s="5">
+      <c r="AR4" s="4">
         <f t="shared" ref="AR4:AR6" si="0">0+AQ4</f>
         <v>0</v>
       </c>
-      <c r="AS4" s="5">
+      <c r="AS4" s="4">
         <f t="shared" ref="AS4:AS6" si="1">((2^AO4)*AP4)+AQ4</f>
         <v>65536</v>
       </c>
-      <c r="AT4" s="5">
+      <c r="AT4" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="A5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="5">
-        <v>4</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>87</v>
-      </c>
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
@@ -2191,9 +2158,9 @@
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="9" t="s">
-        <v>86</v>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="W5" s="10"/>
       <c r="X5" s="10"/>
@@ -2209,58 +2176,111 @@
       <c r="AH5" s="10"/>
       <c r="AI5" s="10"/>
       <c r="AJ5" s="10"/>
-      <c r="AK5" s="11"/>
-      <c r="AN5" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO5" s="5">
-        <v>16</v>
-      </c>
-      <c r="AP5" s="12">
+      <c r="AK5" s="10"/>
+      <c r="AN5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO5" s="4">
+        <v>16</v>
+      </c>
+      <c r="AP5" s="6">
         <v>1</v>
       </c>
-      <c r="AQ5" s="5">
+      <c r="AQ5" s="4">
         <v>0</v>
       </c>
-      <c r="AR5" s="5">
+      <c r="AR5" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AS5" s="5">
+      <c r="AS5" s="4">
         <f t="shared" si="1"/>
         <v>65536</v>
       </c>
-      <c r="AT5" s="5">
+      <c r="AT5" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="AN6" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO6" s="5">
-        <v>16</v>
-      </c>
-      <c r="AP6" s="12">
+      <c r="A6" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
+      <c r="AJ6" s="10"/>
+      <c r="AK6" s="10"/>
+      <c r="AN6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO6" s="4">
+        <v>16</v>
+      </c>
+      <c r="AP6" s="6">
         <v>1</v>
       </c>
-      <c r="AQ6" s="5">
+      <c r="AQ6" s="4">
         <v>0</v>
       </c>
-      <c r="AR6" s="5">
+      <c r="AR6" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AS6" s="5">
+      <c r="AS6" s="4">
         <f t="shared" si="1"/>
         <v>65536</v>
       </c>
-      <c r="AT6" s="5">
+      <c r="AT6" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
+    <mergeCell ref="V5:AK5"/>
+    <mergeCell ref="F5:U5"/>
+    <mergeCell ref="F6:U6"/>
+    <mergeCell ref="V6:AK6"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="N2:U2"/>
     <mergeCell ref="V2:AC2"/>
@@ -2272,8 +2292,6 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="V5:AK5"/>
-    <mergeCell ref="F5:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated pos signals to be 8 bits
</commit_message>
<xml_diff>
--- a/1_Planning/System_Interface_Design.xlsx
+++ b/1_Planning/System_Interface_Design.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="98">
   <si>
     <t>System Interface Design</t>
   </si>
@@ -250,12 +250,6 @@
   </si>
   <si>
     <t>DLC</t>
-  </si>
-  <si>
-    <t>Byte 3</t>
-  </si>
-  <si>
-    <t>Byte 2</t>
   </si>
   <si>
     <t>Byte 1</t>
@@ -369,7 +363,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -392,11 +386,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -413,7 +444,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1818,10 +1855,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT6"/>
+  <dimension ref="A1:AD6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,24 +1867,24 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="6" max="37" width="3.7109375" customWidth="1"/>
-    <col min="40" max="40" width="15.85546875" customWidth="1"/>
-    <col min="41" max="41" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="6" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="21" width="3.7109375" customWidth="1"/>
+    <col min="24" max="24" width="15.85546875" customWidth="1"/>
+    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="6" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:30" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AN1" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="X1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>72</v>
       </c>
@@ -1855,7 +1892,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>73</v>
@@ -1883,49 +1920,29 @@
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
-      <c r="V2" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="8"/>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="8"/>
-      <c r="AK2" s="8"/>
-      <c r="AN2" s="5" t="s">
+      <c r="X2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="AO2" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="AP2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="AQ2" s="5" t="s">
+      <c r="AC2" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="AR2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="AS2" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT2" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1979,81 +1996,33 @@
       <c r="U3" s="5">
         <v>0</v>
       </c>
-      <c r="V3" s="5">
-        <v>7</v>
-      </c>
-      <c r="W3" s="5">
-        <v>6</v>
-      </c>
-      <c r="X3" s="5">
-        <v>5</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>4</v>
-      </c>
-      <c r="Z3" s="5">
-        <v>3</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>2</v>
-      </c>
-      <c r="AB3" s="5">
+      <c r="X3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>8</v>
+      </c>
+      <c r="Z3" s="6">
         <v>1</v>
       </c>
-      <c r="AC3" s="5">
+      <c r="AA3" s="4">
         <v>0</v>
       </c>
-      <c r="AD3" s="5">
-        <v>7</v>
-      </c>
-      <c r="AE3" s="5">
-        <v>6</v>
-      </c>
-      <c r="AF3" s="5">
-        <v>5</v>
-      </c>
-      <c r="AG3" s="5">
-        <v>4</v>
-      </c>
-      <c r="AH3" s="5">
-        <v>3</v>
-      </c>
-      <c r="AI3" s="5">
-        <v>2</v>
-      </c>
-      <c r="AJ3" s="5">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="5">
+      <c r="AB3" s="4">
+        <f>0+AA3</f>
         <v>0</v>
       </c>
-      <c r="AN3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO3" s="4">
-        <v>16</v>
-      </c>
-      <c r="AP3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AQ3" s="4">
+      <c r="AC3" s="4">
+        <f>((2^Y3)*Z3)+AA3</f>
+        <v>256</v>
+      </c>
+      <c r="AD3" s="4">
         <v>0</v>
       </c>
-      <c r="AR3" s="4">
-        <f>0+AQ3</f>
-        <v>0</v>
-      </c>
-      <c r="AS3" s="4">
-        <f>((2^AO3)*AP3)+AQ3</f>
-        <v>65536</v>
-      </c>
-      <c r="AT3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>28</v>
@@ -2062,236 +2031,186 @@
         <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E4" s="4">
         <v>4</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="10"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
-      <c r="AN4" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AO4" s="4">
-        <v>16</v>
-      </c>
-      <c r="AP4" s="6">
+        <v>82</v>
+      </c>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="12"/>
+      <c r="X4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>8</v>
+      </c>
+      <c r="Z4" s="6">
         <v>1</v>
       </c>
-      <c r="AQ4" s="4">
+      <c r="AA4" s="4">
         <v>0</v>
       </c>
-      <c r="AR4" s="4">
-        <f t="shared" ref="AR4:AR6" si="0">0+AQ4</f>
+      <c r="AB4" s="4">
+        <f t="shared" ref="AB4:AB6" si="0">0+AA4</f>
         <v>0</v>
       </c>
-      <c r="AS4" s="4">
-        <f t="shared" ref="AS4:AS6" si="1">((2^AO4)*AP4)+AQ4</f>
-        <v>65536</v>
-      </c>
-      <c r="AT4" s="4">
+      <c r="AC4" s="4">
+        <f t="shared" ref="AC4:AC6" si="1">((2^Y4)*Z4)+AA4</f>
+        <v>256</v>
+      </c>
+      <c r="AD4" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E5" s="4">
         <v>2</v>
       </c>
       <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="10"/>
-      <c r="AB5" s="10"/>
-      <c r="AC5" s="10"/>
-      <c r="AD5" s="10"/>
-      <c r="AE5" s="10"/>
-      <c r="AF5" s="10"/>
-      <c r="AG5" s="10"/>
-      <c r="AH5" s="10"/>
-      <c r="AI5" s="10"/>
-      <c r="AJ5" s="10"/>
-      <c r="AK5" s="10"/>
-      <c r="AN5" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AO5" s="4">
-        <v>16</v>
-      </c>
-      <c r="AP5" s="6">
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="12"/>
+      <c r="X5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>8</v>
+      </c>
+      <c r="Z5" s="6">
         <v>1</v>
       </c>
-      <c r="AQ5" s="4">
+      <c r="AA5" s="4">
         <v>0</v>
       </c>
-      <c r="AR5" s="4">
+      <c r="AB5" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AS5" s="4">
+      <c r="AC5" s="4">
         <f t="shared" si="1"/>
-        <v>65536</v>
-      </c>
-      <c r="AT5" s="4">
+        <v>256</v>
+      </c>
+      <c r="AD5" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E6" s="4">
         <v>2</v>
       </c>
       <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="10"/>
-      <c r="AB6" s="10"/>
-      <c r="AC6" s="10"/>
-      <c r="AD6" s="10"/>
-      <c r="AE6" s="10"/>
-      <c r="AF6" s="10"/>
-      <c r="AG6" s="10"/>
-      <c r="AH6" s="10"/>
-      <c r="AI6" s="10"/>
-      <c r="AJ6" s="10"/>
-      <c r="AK6" s="10"/>
-      <c r="AN6" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO6" s="4">
-        <v>16</v>
-      </c>
-      <c r="AP6" s="6">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="12"/>
+      <c r="X6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y6" s="4">
+        <v>8</v>
+      </c>
+      <c r="Z6" s="6">
         <v>1</v>
       </c>
-      <c r="AQ6" s="4">
+      <c r="AA6" s="4">
         <v>0</v>
       </c>
-      <c r="AR6" s="4">
+      <c r="AB6" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AS6" s="4">
+      <c r="AC6" s="4">
         <f t="shared" si="1"/>
-        <v>65536</v>
-      </c>
-      <c r="AT6" s="4">
+        <v>256</v>
+      </c>
+      <c r="AD6" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="V5:AK5"/>
-    <mergeCell ref="F5:U5"/>
-    <mergeCell ref="F6:U6"/>
-    <mergeCell ref="V6:AK6"/>
+  <mergeCells count="13">
+    <mergeCell ref="N4:U4"/>
+    <mergeCell ref="F5:M5"/>
+    <mergeCell ref="N5:U5"/>
+    <mergeCell ref="F6:M6"/>
+    <mergeCell ref="N6:U6"/>
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="F2:M2"/>
     <mergeCell ref="N2:U2"/>
-    <mergeCell ref="V2:AC2"/>
-    <mergeCell ref="AD2:AK2"/>
-    <mergeCell ref="F4:U4"/>
-    <mergeCell ref="V4:AK4"/>
-    <mergeCell ref="F2:M2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B2:B3"/>
+    <mergeCell ref="F4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated pos signals to be 16 bits
</commit_message>
<xml_diff>
--- a/1_Planning/System_Interface_Design.xlsx
+++ b/1_Planning/System_Interface_Design.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="100">
   <si>
     <t>System Interface Design</t>
   </si>
@@ -319,6 +319,12 @@
   </si>
   <si>
     <t>0x102</t>
+  </si>
+  <si>
+    <t>Byte 2</t>
+  </si>
+  <si>
+    <t>Byte 3</t>
   </si>
 </sst>
 </file>
@@ -435,6 +441,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -443,15 +458,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1855,10 +1861,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD6"/>
+  <dimension ref="A1:AT6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="F6" sqref="F6:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1867,87 +1873,107 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="6" max="21" width="3.7109375" customWidth="1"/>
-    <col min="24" max="24" width="15.85546875" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="6" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="37" width="3.7109375" customWidth="1"/>
+    <col min="40" max="40" width="15.85546875" customWidth="1"/>
+    <col min="41" max="41" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="6" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:46" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
+      <c r="V2" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8" t="s">
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="X2" s="5" t="s">
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="11"/>
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="11"/>
+      <c r="AJ2" s="11"/>
+      <c r="AK2" s="11"/>
+      <c r="AN2" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="AO2" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AP2" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AQ2" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AR2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AS2" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AT2" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="9"/>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="5">
         <v>7</v>
       </c>
@@ -1996,31 +2022,79 @@
       <c r="U3" s="5">
         <v>0</v>
       </c>
-      <c r="X3" s="4" t="s">
+      <c r="V3" s="5">
+        <v>7</v>
+      </c>
+      <c r="W3" s="5">
+        <v>6</v>
+      </c>
+      <c r="X3" s="5">
+        <v>5</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>4</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>3</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="5">
+        <v>7</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>6</v>
+      </c>
+      <c r="AF3" s="5">
+        <v>5</v>
+      </c>
+      <c r="AG3" s="5">
+        <v>4</v>
+      </c>
+      <c r="AH3" s="5">
+        <v>3</v>
+      </c>
+      <c r="AI3" s="5">
+        <v>2</v>
+      </c>
+      <c r="AJ3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="Y3" s="4">
-        <v>8</v>
-      </c>
-      <c r="Z3" s="6">
+      <c r="AO3" s="4">
+        <v>16</v>
+      </c>
+      <c r="AP3" s="6">
         <v>1</v>
       </c>
-      <c r="AA3" s="4">
+      <c r="AQ3" s="4">
         <v>0</v>
       </c>
-      <c r="AB3" s="4">
-        <f>0+AA3</f>
+      <c r="AR3" s="4">
+        <f>0+AQ3</f>
         <v>0</v>
       </c>
-      <c r="AC3" s="4">
-        <f>((2^Y3)*Z3)+AA3</f>
-        <v>256</v>
-      </c>
-      <c r="AD3" s="4">
+      <c r="AS3" s="4">
+        <f>((2^AO3)*AP3)+AQ3</f>
+        <v>65536</v>
+      </c>
+      <c r="AT3" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>80</v>
       </c>
@@ -2036,51 +2110,67 @@
       <c r="E4" s="4">
         <v>4</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="10" t="s">
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="12"/>
-      <c r="X4" s="4" t="s">
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="9"/>
+      <c r="AN4" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="Y4" s="4">
-        <v>8</v>
-      </c>
-      <c r="Z4" s="6">
+      <c r="AO4" s="4">
+        <v>16</v>
+      </c>
+      <c r="AP4" s="6">
         <v>1</v>
       </c>
-      <c r="AA4" s="4">
+      <c r="AQ4" s="4">
         <v>0</v>
       </c>
-      <c r="AB4" s="4">
-        <f t="shared" ref="AB4:AB6" si="0">0+AA4</f>
+      <c r="AR4" s="4">
+        <f t="shared" ref="AR4:AR6" si="0">0+AQ4</f>
         <v>0</v>
       </c>
-      <c r="AC4" s="4">
-        <f t="shared" ref="AC4:AC6" si="1">((2^Y4)*Z4)+AA4</f>
-        <v>256</v>
-      </c>
-      <c r="AD4" s="4">
+      <c r="AS4" s="4">
+        <f t="shared" ref="AS4:AS6" si="1">((2^AO4)*AP4)+AQ4</f>
+        <v>65536</v>
+      </c>
+      <c r="AT4" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>93</v>
       </c>
@@ -2096,49 +2186,65 @@
       <c r="E5" s="4">
         <v>2</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="10" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="12"/>
-      <c r="X5" s="4" t="s">
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8"/>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="8"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
+      <c r="AK5" s="9"/>
+      <c r="AN5" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="Y5" s="4">
-        <v>8</v>
-      </c>
-      <c r="Z5" s="6">
+      <c r="AO5" s="4">
+        <v>16</v>
+      </c>
+      <c r="AP5" s="6">
         <v>1</v>
       </c>
-      <c r="AA5" s="4">
+      <c r="AQ5" s="4">
         <v>0</v>
       </c>
-      <c r="AB5" s="4">
+      <c r="AR5" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AC5" s="4">
+      <c r="AS5" s="4">
         <f t="shared" si="1"/>
-        <v>256</v>
-      </c>
-      <c r="AD5" s="4">
+        <v>65536</v>
+      </c>
+      <c r="AT5" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>94</v>
       </c>
@@ -2154,63 +2260,83 @@
       <c r="E6" s="4">
         <v>2</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="10" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="12"/>
-      <c r="X6" s="4" t="s">
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="9"/>
+      <c r="AN6" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Y6" s="4">
-        <v>8</v>
-      </c>
-      <c r="Z6" s="6">
+      <c r="AO6" s="4">
+        <v>16</v>
+      </c>
+      <c r="AP6" s="6">
         <v>1</v>
       </c>
-      <c r="AA6" s="4">
+      <c r="AQ6" s="4">
         <v>0</v>
       </c>
-      <c r="AB6" s="4">
+      <c r="AR6" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AC6" s="4">
+      <c r="AS6" s="4">
         <f t="shared" si="1"/>
-        <v>256</v>
-      </c>
-      <c r="AD6" s="4">
+        <v>65536</v>
+      </c>
+      <c r="AT6" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="N4:U4"/>
+  <mergeCells count="17">
     <mergeCell ref="F5:M5"/>
     <mergeCell ref="N5:U5"/>
     <mergeCell ref="F6:M6"/>
     <mergeCell ref="N6:U6"/>
+    <mergeCell ref="F4:U4"/>
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="F2:M2"/>
-    <mergeCell ref="N2:U2"/>
+    <mergeCell ref="V2:AC2"/>
+    <mergeCell ref="AD2:AK2"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="F4:M4"/>
+    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="N2:U2"/>
+    <mergeCell ref="V4:AK4"/>
+    <mergeCell ref="V5:AK5"/>
+    <mergeCell ref="V6:AK6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Edited CAN msgs for States and Goal scoring
</commit_message>
<xml_diff>
--- a/1_Planning/System_Interface_Design.xlsx
+++ b/1_Planning/System_Interface_Design.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\capstone\1_Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srashevskyi8178\Desktop\GitHub\capstone\1_Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="110">
   <si>
     <t>System Interface Design</t>
   </si>
@@ -325,6 +325,44 @@
   </si>
   <si>
     <t>Byte 3</t>
+  </si>
+  <si>
+    <t>state_x</t>
+  </si>
+  <si>
+    <t>state_y</t>
+  </si>
+  <si>
+    <t>goal_scored</t>
+  </si>
+  <si>
+    <t># of Bits</t>
+  </si>
+  <si>
+    <t>Value Descriptions</t>
+  </si>
+  <si>
+    <t>0 = Stopped
+1 = Running
+2 = Initializing
+3 = Calibrating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC X-axis signal describing
+ its current state </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC Y-axis signal describing
+ its current state </t>
+  </si>
+  <si>
+    <t>0 = None
+1 = Human scored
+2 = Robot scored</t>
+  </si>
+  <si>
+    <t>PC X-axis signal describing
+whether the goal was scored</t>
   </si>
 </sst>
 </file>
@@ -433,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -441,6 +479,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,6 +506,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1861,10 +1936,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT6"/>
+  <dimension ref="A1:AV12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:M6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,7 +1948,9 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="6" max="37" width="3.7109375" customWidth="1"/>
+    <col min="6" max="17" width="3.7109375" customWidth="1"/>
+    <col min="18" max="21" width="6.7109375" customWidth="1"/>
+    <col min="22" max="37" width="2.7109375" customWidth="1"/>
     <col min="40" max="40" width="15.85546875" customWidth="1"/>
     <col min="41" max="41" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="13.140625" bestFit="1" customWidth="1"/>
@@ -1882,7 +1959,7 @@
     <col min="46" max="46" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:48" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
@@ -1890,62 +1967,62 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11" t="s">
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11" t="s">
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
       <c r="AN2" s="5" t="s">
         <v>86</v>
       </c>
@@ -1959,21 +2036,21 @@
         <v>88</v>
       </c>
       <c r="AR2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS2" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="AS2" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="AT2" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="12"/>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="5">
         <v>7</v>
       </c>
@@ -2094,7 +2171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>80</v>
       </c>
@@ -2110,42 +2187,42 @@
       <c r="E4" s="4">
         <v>4</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="7" t="s">
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="8"/>
-      <c r="AE4" s="8"/>
-      <c r="AF4" s="8"/>
-      <c r="AG4" s="8"/>
-      <c r="AH4" s="8"/>
-      <c r="AI4" s="8"/>
-      <c r="AJ4" s="8"/>
-      <c r="AK4" s="9"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="11"/>
+      <c r="AI4" s="11"/>
+      <c r="AJ4" s="11"/>
+      <c r="AK4" s="12"/>
       <c r="AN4" s="4" t="s">
         <v>82</v>
       </c>
@@ -2170,7 +2247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>93</v>
       </c>
@@ -2186,40 +2263,43 @@
       <c r="E5" s="4">
         <v>2</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="7" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="12"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="U5" s="12"/>
+      <c r="V5" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-      <c r="AC5" s="8"/>
-      <c r="AD5" s="8"/>
-      <c r="AE5" s="8"/>
-      <c r="AF5" s="8"/>
-      <c r="AG5" s="8"/>
-      <c r="AH5" s="8"/>
-      <c r="AI5" s="8"/>
-      <c r="AJ5" s="8"/>
-      <c r="AK5" s="9"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="11"/>
+      <c r="AG5" s="11"/>
+      <c r="AH5" s="11"/>
+      <c r="AI5" s="11"/>
+      <c r="AJ5" s="11"/>
+      <c r="AK5" s="12"/>
       <c r="AN5" s="4" t="s">
         <v>83</v>
       </c>
@@ -2244,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>94</v>
       </c>
@@ -2260,40 +2340,42 @@
       <c r="E6" s="4">
         <v>2</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="12"/>
       <c r="N6" s="7"/>
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
+      <c r="R6" s="7"/>
       <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="7" t="s">
+      <c r="T6" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="U6" s="12"/>
+      <c r="V6" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="8"/>
-      <c r="AB6" s="8"/>
-      <c r="AC6" s="8"/>
-      <c r="AD6" s="8"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="8"/>
-      <c r="AG6" s="8"/>
-      <c r="AH6" s="8"/>
-      <c r="AI6" s="8"/>
-      <c r="AJ6" s="8"/>
-      <c r="AK6" s="9"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="11"/>
+      <c r="AK6" s="12"/>
       <c r="AN6" s="4" t="s">
         <v>84</v>
       </c>
@@ -2318,13 +2400,96 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AN9" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO9" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP9" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="AQ9" s="19"/>
+      <c r="AR9" s="20"/>
+      <c r="AS9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT9" s="19"/>
+      <c r="AU9" s="19"/>
+      <c r="AV9" s="20"/>
+    </row>
+    <row r="10" spans="1:48" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN10" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AO10" s="17">
+        <v>2</v>
+      </c>
+      <c r="AP10" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="AQ10" s="22"/>
+      <c r="AR10" s="22"/>
+      <c r="AS10" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="AT10" s="23"/>
+      <c r="AU10" s="23"/>
+      <c r="AV10" s="24"/>
+    </row>
+    <row r="11" spans="1:48" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN11" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="AO11" s="17">
+        <v>2</v>
+      </c>
+      <c r="AP11" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="AQ11" s="22"/>
+      <c r="AR11" s="22"/>
+      <c r="AS11" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT11" s="23"/>
+      <c r="AU11" s="23"/>
+      <c r="AV11" s="24"/>
+    </row>
+    <row r="12" spans="1:48" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AN12" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="AO12" s="17">
+        <v>2</v>
+      </c>
+      <c r="AP12" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="AQ12" s="22"/>
+      <c r="AR12" s="22"/>
+      <c r="AS12" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="AT12" s="23"/>
+      <c r="AU12" s="23"/>
+      <c r="AV12" s="24"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="F5:M5"/>
-    <mergeCell ref="N5:U5"/>
-    <mergeCell ref="F6:M6"/>
-    <mergeCell ref="N6:U6"/>
-    <mergeCell ref="F4:U4"/>
+  <mergeCells count="26">
+    <mergeCell ref="AP12:AR12"/>
+    <mergeCell ref="AS12:AV12"/>
+    <mergeCell ref="AP11:AR11"/>
+    <mergeCell ref="AS11:AV11"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="AS9:AV9"/>
+    <mergeCell ref="AP9:AR9"/>
+    <mergeCell ref="AP10:AR10"/>
+    <mergeCell ref="AS10:AV10"/>
+    <mergeCell ref="V4:AK4"/>
+    <mergeCell ref="V5:AK5"/>
+    <mergeCell ref="V6:AK6"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="V2:AC2"/>
     <mergeCell ref="AD2:AK2"/>
@@ -2334,9 +2499,11 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="N2:U2"/>
-    <mergeCell ref="V4:AK4"/>
-    <mergeCell ref="V5:AK5"/>
-    <mergeCell ref="V6:AK6"/>
+    <mergeCell ref="F5:M5"/>
+    <mergeCell ref="F6:M6"/>
+    <mergeCell ref="F4:U4"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="R5:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated CAN Protocol signals
</commit_message>
<xml_diff>
--- a/1_Planning/System_Interface_Design.xlsx
+++ b/1_Planning/System_Interface_Design.xlsx
@@ -14,6 +14,8 @@
   <sheets>
     <sheet name="Signal List" sheetId="1" r:id="rId1"/>
     <sheet name="CAN Messages" sheetId="2" r:id="rId2"/>
+    <sheet name="MC_Cmd_PC Signals" sheetId="4" r:id="rId3"/>
+    <sheet name="PC_Status Signals" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="125">
   <si>
     <t>System Interface Design</t>
   </si>
@@ -282,78 +284,19 @@
     <t>pos_y_mm</t>
   </si>
   <si>
-    <t>CAN Signal Descriptions</t>
-  </si>
-  <si>
     <t>Signal Name</t>
   </si>
   <si>
-    <t>Scaling Factor</t>
-  </si>
-  <si>
-    <t>Offset</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Initial Value</t>
-  </si>
-  <si>
     <t>Length (Bits)</t>
   </si>
   <si>
-    <t>PC_Status_X</t>
-  </si>
-  <si>
-    <t>PC_Status_Y</t>
-  </si>
-  <si>
-    <t>PC_Y</t>
-  </si>
-  <si>
-    <t>PC_X</t>
-  </si>
-  <si>
-    <t>0x102</t>
-  </si>
-  <si>
     <t>Byte 2</t>
   </si>
   <si>
     <t>Byte 3</t>
   </si>
   <si>
-    <t>state_x</t>
-  </si>
-  <si>
-    <t>state_y</t>
-  </si>
-  <si>
     <t>goal_scored</t>
-  </si>
-  <si>
-    <t># of Bits</t>
-  </si>
-  <si>
-    <t>Value Descriptions</t>
-  </si>
-  <si>
-    <t>0 = Stopped
-1 = Running
-2 = Initializing
-3 = Calibrating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PC X-axis signal describing
- its current state </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PC Y-axis signal describing
- its current state </t>
   </si>
   <si>
     <t>0 = None
@@ -361,15 +304,132 @@
 2 = Robot scored</t>
   </si>
   <si>
-    <t>PC X-axis signal describing
-whether the goal was scored</t>
+    <t>PC signal describing
+who scored the goal</t>
+  </si>
+  <si>
+    <t>PC_Status</t>
+  </si>
+  <si>
+    <t>motor_speed_x</t>
+  </si>
+  <si>
+    <t>motor_speed_y</t>
+  </si>
+  <si>
+    <t>Byte 4</t>
+  </si>
+  <si>
+    <t>Byte 5</t>
+  </si>
+  <si>
+    <t>Byte 6</t>
+  </si>
+  <si>
+    <t>Byte 7</t>
+  </si>
+  <si>
+    <t>motor_speed_cmd_y</t>
+  </si>
+  <si>
+    <t>motor_speed_cmd_x</t>
+  </si>
+  <si>
+    <t>state_cmd</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>0 = OFF
+1 = Calibration
+2 = ON
+3 = Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC signal with
+ its current state </t>
+  </si>
+  <si>
+    <t>0 = Slow
+1 = Medium
+2 = Fast</t>
+  </si>
+  <si>
+    <t>0 = none
+1 = …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC signal with
+ its current error (if any) </t>
+  </si>
+  <si>
+    <t>*debug (empty)*</t>
+  </si>
+  <si>
+    <t>0 to 65536</t>
+  </si>
+  <si>
+    <t>PC signal with current
+ X-axis motor speed</t>
+  </si>
+  <si>
+    <t>PC signal with current PC
+ Y-axis motor speed</t>
+  </si>
+  <si>
+    <t>PC signal with current X-axis paddle position in mm</t>
+  </si>
+  <si>
+    <t>PC signal with current Y-axis paddle position in mm</t>
+  </si>
+  <si>
+    <t>PC_Status - Signal Descriptions</t>
+  </si>
+  <si>
+    <t>MC_Cmd_PC - Signal Descriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC signal that commands PC to
+ change state </t>
+  </si>
+  <si>
+    <t>0 = OFF
+1 = Calibration
+2 = ON
+3 = Clear_Error</t>
+  </si>
+  <si>
+    <t>MC signal that commands PC to
+ change Y-axis motor speed</t>
+  </si>
+  <si>
+    <t>MC signal that commands PC to
+ change X-axis motor speed</t>
+  </si>
+  <si>
+    <t>MC signal that commands PC to
+ change Y-axis paddle position in mm</t>
+  </si>
+  <si>
+    <t>MC signal that commands PC to
+ change X-axis paddle position in mm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,20 +454,46 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -467,33 +553,98 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -501,17 +652,43 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -521,21 +698,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
+    <cellStyle name="40% - Accent3" xfId="3" builtinId="39"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -816,7 +1017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1936,560 +2139,688 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV12"/>
+  <dimension ref="A1:BQ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="6" max="17" width="3.7109375" customWidth="1"/>
-    <col min="18" max="21" width="6.7109375" customWidth="1"/>
-    <col min="22" max="37" width="2.7109375" customWidth="1"/>
-    <col min="40" max="40" width="15.85546875" customWidth="1"/>
-    <col min="41" max="41" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="6" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="29" width="2.7109375" customWidth="1"/>
+    <col min="30" max="33" width="3.7109375" customWidth="1"/>
+    <col min="34" max="37" width="8.7109375" customWidth="1"/>
+    <col min="38" max="69" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:69" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AN1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    </row>
+    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="14" t="s">
         <v>73</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
+      <c r="AJ2" s="35"/>
+      <c r="AK2" s="35"/>
+      <c r="AL2" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="34"/>
+      <c r="AO2" s="34"/>
+      <c r="AP2" s="34"/>
+      <c r="AQ2" s="34"/>
+      <c r="AR2" s="34"/>
+      <c r="AS2" s="34"/>
+      <c r="AT2" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU2" s="35"/>
+      <c r="AV2" s="35"/>
+      <c r="AW2" s="35"/>
+      <c r="AX2" s="35"/>
+      <c r="AY2" s="35"/>
+      <c r="AZ2" s="35"/>
+      <c r="BA2" s="35"/>
+      <c r="BB2" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC2" s="34"/>
+      <c r="BD2" s="34"/>
+      <c r="BE2" s="34"/>
+      <c r="BF2" s="34"/>
+      <c r="BG2" s="34"/>
+      <c r="BH2" s="34"/>
+      <c r="BI2" s="34"/>
+      <c r="BJ2" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="BK2" s="35"/>
+      <c r="BL2" s="35"/>
+      <c r="BM2" s="35"/>
+      <c r="BN2" s="35"/>
+      <c r="BO2" s="35"/>
+      <c r="BP2" s="35"/>
+      <c r="BQ2" s="35"/>
+    </row>
+    <row r="3" spans="1:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="30">
+        <v>7</v>
+      </c>
+      <c r="G3" s="30">
+        <v>6</v>
+      </c>
+      <c r="H3" s="30">
+        <v>5</v>
+      </c>
+      <c r="I3" s="30">
+        <v>4</v>
+      </c>
+      <c r="J3" s="30">
+        <v>3</v>
+      </c>
+      <c r="K3" s="30">
+        <v>2</v>
+      </c>
+      <c r="L3" s="30">
+        <v>1</v>
+      </c>
+      <c r="M3" s="30">
+        <v>0</v>
+      </c>
+      <c r="N3" s="29">
+        <v>7</v>
+      </c>
+      <c r="O3" s="29">
+        <v>6</v>
+      </c>
+      <c r="P3" s="29">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="29">
+        <v>4</v>
+      </c>
+      <c r="R3" s="29">
+        <v>3</v>
+      </c>
+      <c r="S3" s="29">
+        <v>2</v>
+      </c>
+      <c r="T3" s="29">
+        <v>1</v>
+      </c>
+      <c r="U3" s="29">
+        <v>0</v>
+      </c>
+      <c r="V3" s="30">
+        <v>7</v>
+      </c>
+      <c r="W3" s="30">
+        <v>6</v>
+      </c>
+      <c r="X3" s="30">
+        <v>5</v>
+      </c>
+      <c r="Y3" s="30">
+        <v>4</v>
+      </c>
+      <c r="Z3" s="30">
+        <v>3</v>
+      </c>
+      <c r="AA3" s="30">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="30">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="29">
+        <v>7</v>
+      </c>
+      <c r="AE3" s="29">
+        <v>6</v>
+      </c>
+      <c r="AF3" s="29">
+        <v>5</v>
+      </c>
+      <c r="AG3" s="29">
+        <v>4</v>
+      </c>
+      <c r="AH3" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI3" s="29">
+        <v>2</v>
+      </c>
+      <c r="AJ3" s="29">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="29">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="30">
+        <v>7</v>
+      </c>
+      <c r="AM3" s="30">
+        <v>6</v>
+      </c>
+      <c r="AN3" s="30">
+        <v>5</v>
+      </c>
+      <c r="AO3" s="30">
+        <v>4</v>
+      </c>
+      <c r="AP3" s="30">
+        <v>3</v>
+      </c>
+      <c r="AQ3" s="30">
+        <v>2</v>
+      </c>
+      <c r="AR3" s="30">
+        <v>1</v>
+      </c>
+      <c r="AS3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="29">
+        <v>7</v>
+      </c>
+      <c r="AU3" s="29">
+        <v>6</v>
+      </c>
+      <c r="AV3" s="29">
+        <v>5</v>
+      </c>
+      <c r="AW3" s="29">
+        <v>4</v>
+      </c>
+      <c r="AX3" s="29">
+        <v>3</v>
+      </c>
+      <c r="AY3" s="29">
+        <v>2</v>
+      </c>
+      <c r="AZ3" s="29">
+        <v>1</v>
+      </c>
+      <c r="BA3" s="29">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="30">
+        <v>7</v>
+      </c>
+      <c r="BC3" s="30">
+        <v>6</v>
+      </c>
+      <c r="BD3" s="30">
+        <v>5</v>
+      </c>
+      <c r="BE3" s="30">
+        <v>4</v>
+      </c>
+      <c r="BF3" s="30">
+        <v>3</v>
+      </c>
+      <c r="BG3" s="30">
+        <v>2</v>
+      </c>
+      <c r="BH3" s="30">
+        <v>1</v>
+      </c>
+      <c r="BI3" s="30">
+        <v>0</v>
+      </c>
+      <c r="BJ3" s="29">
+        <v>7</v>
+      </c>
+      <c r="BK3" s="29">
+        <v>6</v>
+      </c>
+      <c r="BL3" s="29">
+        <v>5</v>
+      </c>
+      <c r="BM3" s="29">
+        <v>4</v>
+      </c>
+      <c r="BN3" s="29">
+        <v>3</v>
+      </c>
+      <c r="BO3" s="29">
+        <v>2</v>
+      </c>
+      <c r="BP3" s="29">
+        <v>1</v>
+      </c>
+      <c r="BQ3" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:69" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="19">
+        <v>8</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="21"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="21"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="40"/>
+      <c r="AE4" s="40"/>
+      <c r="AF4" s="40"/>
+      <c r="AG4" s="40"/>
+      <c r="AH4" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="14"/>
-      <c r="AG2" s="14"/>
-      <c r="AH2" s="14"/>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="14"/>
-      <c r="AK2" s="14"/>
-      <c r="AN2" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO2" s="5" t="s">
+      <c r="AI4" s="24"/>
+      <c r="AJ4" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK4" s="24"/>
+      <c r="AL4" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM4" s="21"/>
+      <c r="AN4" s="21"/>
+      <c r="AO4" s="21"/>
+      <c r="AP4" s="21"/>
+      <c r="AQ4" s="21"/>
+      <c r="AR4" s="21"/>
+      <c r="AS4" s="21"/>
+      <c r="AT4" s="21"/>
+      <c r="AU4" s="21"/>
+      <c r="AV4" s="21"/>
+      <c r="AW4" s="21"/>
+      <c r="AX4" s="21"/>
+      <c r="AY4" s="21"/>
+      <c r="AZ4" s="21"/>
+      <c r="BA4" s="22"/>
+      <c r="BB4" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="BC4" s="21"/>
+      <c r="BD4" s="21"/>
+      <c r="BE4" s="21"/>
+      <c r="BF4" s="21"/>
+      <c r="BG4" s="21"/>
+      <c r="BH4" s="21"/>
+      <c r="BI4" s="21"/>
+      <c r="BJ4" s="21"/>
+      <c r="BK4" s="21"/>
+      <c r="BL4" s="21"/>
+      <c r="BM4" s="21"/>
+      <c r="BN4" s="21"/>
+      <c r="BO4" s="21"/>
+      <c r="BP4" s="21"/>
+      <c r="BQ4" s="22"/>
+    </row>
+    <row r="5" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="AP2" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ2" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="AR2" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AS2" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="AT2" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="5">
-        <v>7</v>
-      </c>
-      <c r="G3" s="5">
-        <v>6</v>
-      </c>
-      <c r="H3" s="5">
-        <v>5</v>
-      </c>
-      <c r="I3" s="5">
-        <v>4</v>
-      </c>
-      <c r="J3" s="5">
-        <v>3</v>
-      </c>
-      <c r="K3" s="5">
-        <v>2</v>
-      </c>
-      <c r="L3" s="5">
-        <v>1</v>
-      </c>
-      <c r="M3" s="5">
-        <v>0</v>
-      </c>
-      <c r="N3" s="5">
-        <v>7</v>
-      </c>
-      <c r="O3" s="5">
-        <v>6</v>
-      </c>
-      <c r="P3" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>4</v>
-      </c>
-      <c r="R3" s="5">
-        <v>3</v>
-      </c>
-      <c r="S3" s="5">
-        <v>2</v>
-      </c>
-      <c r="T3" s="5">
-        <v>1</v>
-      </c>
-      <c r="U3" s="5">
-        <v>0</v>
-      </c>
-      <c r="V3" s="5">
-        <v>7</v>
-      </c>
-      <c r="W3" s="5">
-        <v>6</v>
-      </c>
-      <c r="X3" s="5">
-        <v>5</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>4</v>
-      </c>
-      <c r="Z3" s="5">
-        <v>3</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>2</v>
-      </c>
-      <c r="AB3" s="5">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="5">
-        <v>7</v>
-      </c>
-      <c r="AE3" s="5">
-        <v>6</v>
-      </c>
-      <c r="AF3" s="5">
-        <v>5</v>
-      </c>
-      <c r="AG3" s="5">
-        <v>4</v>
-      </c>
-      <c r="AH3" s="5">
-        <v>3</v>
-      </c>
-      <c r="AI3" s="5">
-        <v>2</v>
-      </c>
-      <c r="AJ3" s="5">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AO3" s="4">
+      <c r="B5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="AP3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AQ3" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="4">
-        <f>0+AQ3</f>
-        <v>0</v>
-      </c>
-      <c r="AS3" s="4">
-        <f>((2^AO3)*AP3)+AQ3</f>
-        <v>65536</v>
-      </c>
-      <c r="AT3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="4">
-        <v>4</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="11"/>
-      <c r="AH4" s="11"/>
-      <c r="AI4" s="11"/>
-      <c r="AJ4" s="11"/>
-      <c r="AK4" s="12"/>
-      <c r="AN4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO4" s="4">
-        <v>16</v>
-      </c>
-      <c r="AP4" s="6">
-        <v>1</v>
-      </c>
-      <c r="AQ4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="4">
-        <f t="shared" ref="AR4:AR6" si="0">0+AQ4</f>
-        <v>0</v>
-      </c>
-      <c r="AS4" s="4">
-        <f t="shared" ref="AS4:AS6" si="1">((2^AO4)*AP4)+AQ4</f>
-        <v>65536</v>
-      </c>
-      <c r="AT4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>78</v>
       </c>
       <c r="E5" s="4">
-        <v>2</v>
-      </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="12"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11" t="s">
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI5" s="17"/>
+      <c r="AJ5" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="U5" s="12"/>
-      <c r="V5" s="10" t="s">
+      <c r="AK5" s="17"/>
+      <c r="AL5" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM5" s="12"/>
+      <c r="AN5" s="12"/>
+      <c r="AO5" s="12"/>
+      <c r="AP5" s="12"/>
+      <c r="AQ5" s="12"/>
+      <c r="AR5" s="12"/>
+      <c r="AS5" s="12"/>
+      <c r="AT5" s="12"/>
+      <c r="AU5" s="12"/>
+      <c r="AV5" s="12"/>
+      <c r="AW5" s="12"/>
+      <c r="AX5" s="12"/>
+      <c r="AY5" s="12"/>
+      <c r="AZ5" s="12"/>
+      <c r="BA5" s="13"/>
+      <c r="BB5" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
-      <c r="AB5" s="11"/>
-      <c r="AC5" s="11"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="11"/>
-      <c r="AG5" s="11"/>
-      <c r="AH5" s="11"/>
-      <c r="AI5" s="11"/>
-      <c r="AJ5" s="11"/>
-      <c r="AK5" s="12"/>
-      <c r="AN5" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO5" s="4">
-        <v>16</v>
-      </c>
-      <c r="AP5" s="6">
-        <v>1</v>
-      </c>
-      <c r="AQ5" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR5" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AS5" s="4">
-        <f t="shared" si="1"/>
-        <v>65536</v>
-      </c>
-      <c r="AT5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="4">
-        <v>2</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="U6" s="12"/>
-      <c r="V6" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="11"/>
-      <c r="AG6" s="11"/>
-      <c r="AH6" s="11"/>
-      <c r="AI6" s="11"/>
-      <c r="AJ6" s="11"/>
-      <c r="AK6" s="12"/>
-      <c r="AN6" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AO6" s="4">
-        <v>16</v>
-      </c>
-      <c r="AP6" s="6">
-        <v>1</v>
-      </c>
-      <c r="AQ6" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AS6" s="4">
-        <f t="shared" si="1"/>
-        <v>65536</v>
-      </c>
-      <c r="AT6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
-      <c r="AN9" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO9" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="AP9" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="AQ9" s="19"/>
-      <c r="AR9" s="20"/>
-      <c r="AS9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="AT9" s="19"/>
-      <c r="AU9" s="19"/>
-      <c r="AV9" s="20"/>
-    </row>
-    <row r="10" spans="1:48" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AN10" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="AO10" s="17">
-        <v>2</v>
-      </c>
-      <c r="AP10" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="AQ10" s="22"/>
-      <c r="AR10" s="22"/>
-      <c r="AS10" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="AT10" s="23"/>
-      <c r="AU10" s="23"/>
-      <c r="AV10" s="24"/>
-    </row>
-    <row r="11" spans="1:48" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AN11" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="AO11" s="17">
-        <v>2</v>
-      </c>
-      <c r="AP11" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="AQ11" s="22"/>
-      <c r="AR11" s="22"/>
-      <c r="AS11" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="AT11" s="23"/>
-      <c r="AU11" s="23"/>
-      <c r="AV11" s="24"/>
-    </row>
-    <row r="12" spans="1:48" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AN12" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO12" s="17">
-        <v>2</v>
-      </c>
-      <c r="AP12" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="AQ12" s="22"/>
-      <c r="AR12" s="22"/>
-      <c r="AS12" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="AT12" s="23"/>
-      <c r="AU12" s="23"/>
-      <c r="AV12" s="24"/>
-    </row>
+      <c r="BC5" s="12"/>
+      <c r="BD5" s="12"/>
+      <c r="BE5" s="12"/>
+      <c r="BF5" s="12"/>
+      <c r="BG5" s="12"/>
+      <c r="BH5" s="12"/>
+      <c r="BI5" s="12"/>
+      <c r="BJ5" s="12"/>
+      <c r="BK5" s="12"/>
+      <c r="BL5" s="12"/>
+      <c r="BM5" s="12"/>
+      <c r="BN5" s="12"/>
+      <c r="BO5" s="12"/>
+      <c r="BP5" s="12"/>
+      <c r="BQ5" s="13"/>
+    </row>
+    <row r="6" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="27"/>
+      <c r="Y6" s="27"/>
+      <c r="Z6" s="27"/>
+      <c r="AA6" s="27"/>
+      <c r="AB6" s="27"/>
+      <c r="AC6" s="27"/>
+      <c r="AD6" s="28"/>
+      <c r="AE6" s="28"/>
+      <c r="AF6" s="28"/>
+      <c r="AG6" s="28"/>
+      <c r="AH6" s="28"/>
+      <c r="AI6" s="28"/>
+      <c r="AJ6" s="28"/>
+      <c r="AK6" s="28"/>
+      <c r="AL6" s="27"/>
+      <c r="AM6" s="27"/>
+      <c r="AN6" s="27"/>
+      <c r="AO6" s="27"/>
+      <c r="AP6" s="27"/>
+      <c r="AQ6" s="27"/>
+      <c r="AR6" s="27"/>
+      <c r="AS6" s="27"/>
+      <c r="AT6" s="26"/>
+      <c r="AU6" s="27"/>
+      <c r="AV6" s="27"/>
+      <c r="AW6" s="27"/>
+      <c r="AX6" s="26"/>
+      <c r="AY6" s="26"/>
+      <c r="AZ6" s="26"/>
+      <c r="BA6" s="26"/>
+      <c r="BB6" s="27"/>
+      <c r="BC6" s="27"/>
+      <c r="BD6" s="27"/>
+      <c r="BE6" s="27"/>
+      <c r="BF6" s="27"/>
+      <c r="BG6" s="27"/>
+      <c r="BH6" s="27"/>
+      <c r="BI6" s="27"/>
+      <c r="BJ6" s="28"/>
+      <c r="BK6" s="28"/>
+      <c r="BL6" s="28"/>
+      <c r="BM6" s="28"/>
+      <c r="BN6" s="28"/>
+      <c r="BO6" s="28"/>
+      <c r="BP6" s="28"/>
+      <c r="BQ6" s="28"/>
+    </row>
+    <row r="7" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="28"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="28"/>
+      <c r="AB7" s="28"/>
+      <c r="AC7" s="28"/>
+      <c r="AD7" s="28"/>
+      <c r="AE7" s="28"/>
+      <c r="AF7" s="28"/>
+      <c r="AG7" s="28"/>
+      <c r="AH7" s="28"/>
+      <c r="AI7" s="28"/>
+      <c r="AJ7" s="28"/>
+      <c r="AK7" s="28"/>
+      <c r="AL7" s="28"/>
+      <c r="AM7" s="28"/>
+      <c r="AN7" s="28"/>
+      <c r="AO7" s="28"/>
+      <c r="AP7" s="28"/>
+      <c r="AQ7" s="28"/>
+      <c r="AR7" s="28"/>
+      <c r="AS7" s="28"/>
+      <c r="AT7" s="28"/>
+      <c r="AU7" s="28"/>
+      <c r="AV7" s="28"/>
+      <c r="AW7" s="28"/>
+      <c r="AX7" s="28"/>
+      <c r="AY7" s="28"/>
+      <c r="AZ7" s="28"/>
+      <c r="BA7" s="28"/>
+      <c r="BB7" s="28"/>
+      <c r="BC7" s="28"/>
+      <c r="BD7" s="28"/>
+      <c r="BE7" s="28"/>
+      <c r="BF7" s="28"/>
+      <c r="BG7" s="28"/>
+      <c r="BH7" s="28"/>
+      <c r="BI7" s="28"/>
+      <c r="BJ7" s="28"/>
+      <c r="BK7" s="28"/>
+      <c r="BL7" s="28"/>
+      <c r="BM7" s="28"/>
+      <c r="BN7" s="28"/>
+      <c r="BO7" s="28"/>
+      <c r="BP7" s="28"/>
+      <c r="BQ7" s="28"/>
+    </row>
+    <row r="10" spans="1:69" ht="66.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:69" ht="69" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:69" ht="81.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:69" ht="93" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="AP12:AR12"/>
-    <mergeCell ref="AS12:AV12"/>
-    <mergeCell ref="AP11:AR11"/>
-    <mergeCell ref="AS11:AV11"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="AS9:AV9"/>
-    <mergeCell ref="AP9:AR9"/>
-    <mergeCell ref="AP10:AR10"/>
-    <mergeCell ref="AS10:AV10"/>
-    <mergeCell ref="V4:AK4"/>
-    <mergeCell ref="V5:AK5"/>
-    <mergeCell ref="V6:AK6"/>
+  <mergeCells count="37">
+    <mergeCell ref="BJ6:BM6"/>
+    <mergeCell ref="BN6:BQ6"/>
+    <mergeCell ref="AL7:BA7"/>
+    <mergeCell ref="BB7:BQ7"/>
+    <mergeCell ref="BB5:BQ5"/>
+    <mergeCell ref="AL2:AS2"/>
+    <mergeCell ref="AT2:BA2"/>
+    <mergeCell ref="BB2:BI2"/>
+    <mergeCell ref="BJ2:BQ2"/>
+    <mergeCell ref="AL4:BA4"/>
+    <mergeCell ref="BB4:BQ4"/>
+    <mergeCell ref="F7:U7"/>
+    <mergeCell ref="AD5:AG5"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="V4:AC4"/>
+    <mergeCell ref="F4:M4"/>
+    <mergeCell ref="N4:U4"/>
+    <mergeCell ref="V5:AC5"/>
+    <mergeCell ref="N5:U5"/>
+    <mergeCell ref="F5:M5"/>
+    <mergeCell ref="AJ4:AK4"/>
+    <mergeCell ref="AH4:AI4"/>
+    <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="V2:AC2"/>
     <mergeCell ref="AD2:AK2"/>
@@ -2499,13 +2830,366 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="N2:U2"/>
-    <mergeCell ref="F5:M5"/>
-    <mergeCell ref="F6:M6"/>
-    <mergeCell ref="F4:U4"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="AD6:AG6"/>
+    <mergeCell ref="AH6:AK6"/>
+    <mergeCell ref="V7:AK7"/>
+    <mergeCell ref="AL5:BA5"/>
+    <mergeCell ref="AJ5:AK5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="6">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="44"/>
+    </row>
+    <row r="5" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="6">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="6">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="6">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="6">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="6">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="6">
+        <v>4</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="6">
+        <v>4</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added PC State Machine, Updated CAN protocol
</commit_message>
<xml_diff>
--- a/1_Planning/System_Interface_Design.xlsx
+++ b/1_Planning/System_Interface_Design.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\capstone\1_Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srashevskyi8178\Desktop\GitHub\capstone\1_Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,8 @@
   <sheets>
     <sheet name="Signal List" sheetId="1" r:id="rId1"/>
     <sheet name="CAN Messages" sheetId="2" r:id="rId2"/>
+    <sheet name="MC_Cmd_PC Signals" sheetId="4" r:id="rId3"/>
+    <sheet name="PC_Status Signals" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="125">
   <si>
     <t>System Interface Design</t>
   </si>
@@ -282,56 +284,152 @@
     <t>pos_y_mm</t>
   </si>
   <si>
-    <t>CAN Signal Descriptions</t>
-  </si>
-  <si>
     <t>Signal Name</t>
   </si>
   <si>
-    <t>Scaling Factor</t>
-  </si>
-  <si>
-    <t>Offset</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Initial Value</t>
-  </si>
-  <si>
     <t>Length (Bits)</t>
   </si>
   <si>
-    <t>PC_Status_X</t>
-  </si>
-  <si>
-    <t>PC_Status_Y</t>
-  </si>
-  <si>
-    <t>PC_Y</t>
-  </si>
-  <si>
-    <t>PC_X</t>
-  </si>
-  <si>
-    <t>0x102</t>
-  </si>
-  <si>
     <t>Byte 2</t>
   </si>
   <si>
     <t>Byte 3</t>
+  </si>
+  <si>
+    <t>goal_scored</t>
+  </si>
+  <si>
+    <t>0 = None
+1 = Human scored
+2 = Robot scored</t>
+  </si>
+  <si>
+    <t>PC signal describing
+who scored the goal</t>
+  </si>
+  <si>
+    <t>PC_Status</t>
+  </si>
+  <si>
+    <t>motor_speed_x</t>
+  </si>
+  <si>
+    <t>motor_speed_y</t>
+  </si>
+  <si>
+    <t>Byte 4</t>
+  </si>
+  <si>
+    <t>Byte 5</t>
+  </si>
+  <si>
+    <t>Byte 6</t>
+  </si>
+  <si>
+    <t>Byte 7</t>
+  </si>
+  <si>
+    <t>motor_speed_cmd_y</t>
+  </si>
+  <si>
+    <t>motor_speed_cmd_x</t>
+  </si>
+  <si>
+    <t>state_cmd</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>0 = OFF
+1 = Calibration
+2 = ON
+3 = Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC signal with
+ its current state </t>
+  </si>
+  <si>
+    <t>0 = Slow
+1 = Medium
+2 = Fast</t>
+  </si>
+  <si>
+    <t>0 = none
+1 = …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC signal with
+ its current error (if any) </t>
+  </si>
+  <si>
+    <t>*debug (empty)*</t>
+  </si>
+  <si>
+    <t>0 to 65536</t>
+  </si>
+  <si>
+    <t>PC signal with current
+ X-axis motor speed</t>
+  </si>
+  <si>
+    <t>PC signal with current PC
+ Y-axis motor speed</t>
+  </si>
+  <si>
+    <t>PC signal with current X-axis paddle position in mm</t>
+  </si>
+  <si>
+    <t>PC signal with current Y-axis paddle position in mm</t>
+  </si>
+  <si>
+    <t>PC_Status - Signal Descriptions</t>
+  </si>
+  <si>
+    <t>MC_Cmd_PC - Signal Descriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MC signal that commands PC to
+ change state </t>
+  </si>
+  <si>
+    <t>0 = OFF
+1 = Calibration
+2 = ON
+3 = Clear_Error</t>
+  </si>
+  <si>
+    <t>MC signal that commands PC to
+ change Y-axis motor speed</t>
+  </si>
+  <si>
+    <t>MC signal that commands PC to
+ change X-axis motor speed</t>
+  </si>
+  <si>
+    <t>MC signal that commands PC to
+ change Y-axis paddle position in mm</t>
+  </si>
+  <si>
+    <t>MC signal that commands PC to
+ change X-axis paddle position in mm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,20 +454,46 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -429,18 +553,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -454,13 +652,91 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
+    <cellStyle name="40% - Accent3" xfId="3" builtinId="39"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -741,7 +1017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1861,470 +2139,688 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT6"/>
+  <dimension ref="A1:BQ13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:M6"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="5.140625" customWidth="1"/>
-    <col min="6" max="37" width="3.7109375" customWidth="1"/>
-    <col min="40" max="40" width="15.85546875" customWidth="1"/>
-    <col min="41" max="41" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="6" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="29" width="2.7109375" customWidth="1"/>
+    <col min="30" max="33" width="3.7109375" customWidth="1"/>
+    <col min="34" max="37" width="8.7109375" customWidth="1"/>
+    <col min="38" max="69" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:69" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AN1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    </row>
+    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="W2" s="37"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
+      <c r="AJ2" s="35"/>
+      <c r="AK2" s="35"/>
+      <c r="AL2" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM2" s="34"/>
+      <c r="AN2" s="34"/>
+      <c r="AO2" s="34"/>
+      <c r="AP2" s="34"/>
+      <c r="AQ2" s="34"/>
+      <c r="AR2" s="34"/>
+      <c r="AS2" s="34"/>
+      <c r="AT2" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU2" s="35"/>
+      <c r="AV2" s="35"/>
+      <c r="AW2" s="35"/>
+      <c r="AX2" s="35"/>
+      <c r="AY2" s="35"/>
+      <c r="AZ2" s="35"/>
+      <c r="BA2" s="35"/>
+      <c r="BB2" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="BC2" s="34"/>
+      <c r="BD2" s="34"/>
+      <c r="BE2" s="34"/>
+      <c r="BF2" s="34"/>
+      <c r="BG2" s="34"/>
+      <c r="BH2" s="34"/>
+      <c r="BI2" s="34"/>
+      <c r="BJ2" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="BK2" s="35"/>
+      <c r="BL2" s="35"/>
+      <c r="BM2" s="35"/>
+      <c r="BN2" s="35"/>
+      <c r="BO2" s="35"/>
+      <c r="BP2" s="35"/>
+      <c r="BQ2" s="35"/>
+    </row>
+    <row r="3" spans="1:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="30">
+        <v>7</v>
+      </c>
+      <c r="G3" s="30">
+        <v>6</v>
+      </c>
+      <c r="H3" s="30">
+        <v>5</v>
+      </c>
+      <c r="I3" s="30">
+        <v>4</v>
+      </c>
+      <c r="J3" s="30">
+        <v>3</v>
+      </c>
+      <c r="K3" s="30">
+        <v>2</v>
+      </c>
+      <c r="L3" s="30">
+        <v>1</v>
+      </c>
+      <c r="M3" s="30">
+        <v>0</v>
+      </c>
+      <c r="N3" s="29">
+        <v>7</v>
+      </c>
+      <c r="O3" s="29">
+        <v>6</v>
+      </c>
+      <c r="P3" s="29">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="29">
+        <v>4</v>
+      </c>
+      <c r="R3" s="29">
+        <v>3</v>
+      </c>
+      <c r="S3" s="29">
+        <v>2</v>
+      </c>
+      <c r="T3" s="29">
+        <v>1</v>
+      </c>
+      <c r="U3" s="29">
+        <v>0</v>
+      </c>
+      <c r="V3" s="30">
+        <v>7</v>
+      </c>
+      <c r="W3" s="30">
+        <v>6</v>
+      </c>
+      <c r="X3" s="30">
+        <v>5</v>
+      </c>
+      <c r="Y3" s="30">
+        <v>4</v>
+      </c>
+      <c r="Z3" s="30">
+        <v>3</v>
+      </c>
+      <c r="AA3" s="30">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="30">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="29">
+        <v>7</v>
+      </c>
+      <c r="AE3" s="29">
+        <v>6</v>
+      </c>
+      <c r="AF3" s="29">
+        <v>5</v>
+      </c>
+      <c r="AG3" s="29">
+        <v>4</v>
+      </c>
+      <c r="AH3" s="29">
+        <v>3</v>
+      </c>
+      <c r="AI3" s="29">
+        <v>2</v>
+      </c>
+      <c r="AJ3" s="29">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="29">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="30">
+        <v>7</v>
+      </c>
+      <c r="AM3" s="30">
+        <v>6</v>
+      </c>
+      <c r="AN3" s="30">
+        <v>5</v>
+      </c>
+      <c r="AO3" s="30">
+        <v>4</v>
+      </c>
+      <c r="AP3" s="30">
+        <v>3</v>
+      </c>
+      <c r="AQ3" s="30">
+        <v>2</v>
+      </c>
+      <c r="AR3" s="30">
+        <v>1</v>
+      </c>
+      <c r="AS3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="29">
+        <v>7</v>
+      </c>
+      <c r="AU3" s="29">
+        <v>6</v>
+      </c>
+      <c r="AV3" s="29">
+        <v>5</v>
+      </c>
+      <c r="AW3" s="29">
+        <v>4</v>
+      </c>
+      <c r="AX3" s="29">
+        <v>3</v>
+      </c>
+      <c r="AY3" s="29">
+        <v>2</v>
+      </c>
+      <c r="AZ3" s="29">
+        <v>1</v>
+      </c>
+      <c r="BA3" s="29">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="30">
+        <v>7</v>
+      </c>
+      <c r="BC3" s="30">
+        <v>6</v>
+      </c>
+      <c r="BD3" s="30">
+        <v>5</v>
+      </c>
+      <c r="BE3" s="30">
+        <v>4</v>
+      </c>
+      <c r="BF3" s="30">
+        <v>3</v>
+      </c>
+      <c r="BG3" s="30">
+        <v>2</v>
+      </c>
+      <c r="BH3" s="30">
+        <v>1</v>
+      </c>
+      <c r="BI3" s="30">
+        <v>0</v>
+      </c>
+      <c r="BJ3" s="29">
+        <v>7</v>
+      </c>
+      <c r="BK3" s="29">
+        <v>6</v>
+      </c>
+      <c r="BL3" s="29">
+        <v>5</v>
+      </c>
+      <c r="BM3" s="29">
+        <v>4</v>
+      </c>
+      <c r="BN3" s="29">
+        <v>3</v>
+      </c>
+      <c r="BO3" s="29">
+        <v>2</v>
+      </c>
+      <c r="BP3" s="29">
+        <v>1</v>
+      </c>
+      <c r="BQ3" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:69" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="19">
+        <v>8</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
+      <c r="Q4" s="39"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="39"/>
+      <c r="T4" s="39"/>
+      <c r="U4" s="39"/>
+      <c r="V4" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="21"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="21"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="40"/>
+      <c r="AE4" s="40"/>
+      <c r="AF4" s="40"/>
+      <c r="AG4" s="40"/>
+      <c r="AH4" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AN2" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="AO2" s="5" t="s">
+      <c r="AI4" s="24"/>
+      <c r="AJ4" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK4" s="24"/>
+      <c r="AL4" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM4" s="21"/>
+      <c r="AN4" s="21"/>
+      <c r="AO4" s="21"/>
+      <c r="AP4" s="21"/>
+      <c r="AQ4" s="21"/>
+      <c r="AR4" s="21"/>
+      <c r="AS4" s="21"/>
+      <c r="AT4" s="21"/>
+      <c r="AU4" s="21"/>
+      <c r="AV4" s="21"/>
+      <c r="AW4" s="21"/>
+      <c r="AX4" s="21"/>
+      <c r="AY4" s="21"/>
+      <c r="AZ4" s="21"/>
+      <c r="BA4" s="22"/>
+      <c r="BB4" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="BC4" s="21"/>
+      <c r="BD4" s="21"/>
+      <c r="BE4" s="21"/>
+      <c r="BF4" s="21"/>
+      <c r="BG4" s="21"/>
+      <c r="BH4" s="21"/>
+      <c r="BI4" s="21"/>
+      <c r="BJ4" s="21"/>
+      <c r="BK4" s="21"/>
+      <c r="BL4" s="21"/>
+      <c r="BM4" s="21"/>
+      <c r="BN4" s="21"/>
+      <c r="BO4" s="21"/>
+      <c r="BP4" s="21"/>
+      <c r="BQ4" s="22"/>
+    </row>
+    <row r="5" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="AP2" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AQ2" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="AR2" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="AS2" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="AT2" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="5">
-        <v>7</v>
-      </c>
-      <c r="G3" s="5">
-        <v>6</v>
-      </c>
-      <c r="H3" s="5">
-        <v>5</v>
-      </c>
-      <c r="I3" s="5">
-        <v>4</v>
-      </c>
-      <c r="J3" s="5">
-        <v>3</v>
-      </c>
-      <c r="K3" s="5">
-        <v>2</v>
-      </c>
-      <c r="L3" s="5">
-        <v>1</v>
-      </c>
-      <c r="M3" s="5">
-        <v>0</v>
-      </c>
-      <c r="N3" s="5">
-        <v>7</v>
-      </c>
-      <c r="O3" s="5">
-        <v>6</v>
-      </c>
-      <c r="P3" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>4</v>
-      </c>
-      <c r="R3" s="5">
-        <v>3</v>
-      </c>
-      <c r="S3" s="5">
-        <v>2</v>
-      </c>
-      <c r="T3" s="5">
-        <v>1</v>
-      </c>
-      <c r="U3" s="5">
-        <v>0</v>
-      </c>
-      <c r="V3" s="5">
-        <v>7</v>
-      </c>
-      <c r="W3" s="5">
-        <v>6</v>
-      </c>
-      <c r="X3" s="5">
-        <v>5</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>4</v>
-      </c>
-      <c r="Z3" s="5">
-        <v>3</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>2</v>
-      </c>
-      <c r="AB3" s="5">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="5">
-        <v>7</v>
-      </c>
-      <c r="AE3" s="5">
-        <v>6</v>
-      </c>
-      <c r="AF3" s="5">
-        <v>5</v>
-      </c>
-      <c r="AG3" s="5">
-        <v>4</v>
-      </c>
-      <c r="AH3" s="5">
-        <v>3</v>
-      </c>
-      <c r="AI3" s="5">
-        <v>2</v>
-      </c>
-      <c r="AJ3" s="5">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AO3" s="4">
+      <c r="B5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="AP3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AQ3" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="4">
-        <f>0+AQ3</f>
-        <v>0</v>
-      </c>
-      <c r="AS3" s="4">
-        <f>((2^AO3)*AP3)+AQ3</f>
-        <v>65536</v>
-      </c>
-      <c r="AT3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="4">
-        <v>4</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="8"/>
-      <c r="AC4" s="8"/>
-      <c r="AD4" s="8"/>
-      <c r="AE4" s="8"/>
-      <c r="AF4" s="8"/>
-      <c r="AG4" s="8"/>
-      <c r="AH4" s="8"/>
-      <c r="AI4" s="8"/>
-      <c r="AJ4" s="8"/>
-      <c r="AK4" s="9"/>
-      <c r="AN4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AO4" s="4">
-        <v>16</v>
-      </c>
-      <c r="AP4" s="6">
-        <v>1</v>
-      </c>
-      <c r="AQ4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="4">
-        <f t="shared" ref="AR4:AR6" si="0">0+AQ4</f>
-        <v>0</v>
-      </c>
-      <c r="AS4" s="4">
-        <f t="shared" ref="AS4:AS6" si="1">((2^AO4)*AP4)+AQ4</f>
-        <v>65536</v>
-      </c>
-      <c r="AT4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>78</v>
       </c>
       <c r="E5" s="4">
-        <v>2</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI5" s="17"/>
+      <c r="AJ5" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK5" s="17"/>
+      <c r="AL5" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM5" s="12"/>
+      <c r="AN5" s="12"/>
+      <c r="AO5" s="12"/>
+      <c r="AP5" s="12"/>
+      <c r="AQ5" s="12"/>
+      <c r="AR5" s="12"/>
+      <c r="AS5" s="12"/>
+      <c r="AT5" s="12"/>
+      <c r="AU5" s="12"/>
+      <c r="AV5" s="12"/>
+      <c r="AW5" s="12"/>
+      <c r="AX5" s="12"/>
+      <c r="AY5" s="12"/>
+      <c r="AZ5" s="12"/>
+      <c r="BA5" s="13"/>
+      <c r="BB5" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8"/>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8"/>
-      <c r="AC5" s="8"/>
-      <c r="AD5" s="8"/>
-      <c r="AE5" s="8"/>
-      <c r="AF5" s="8"/>
-      <c r="AG5" s="8"/>
-      <c r="AH5" s="8"/>
-      <c r="AI5" s="8"/>
-      <c r="AJ5" s="8"/>
-      <c r="AK5" s="9"/>
-      <c r="AN5" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AO5" s="4">
-        <v>16</v>
-      </c>
-      <c r="AP5" s="6">
-        <v>1</v>
-      </c>
-      <c r="AQ5" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR5" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AS5" s="4">
-        <f t="shared" si="1"/>
-        <v>65536</v>
-      </c>
-      <c r="AT5" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" s="4">
-        <v>2</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-      <c r="AA6" s="8"/>
-      <c r="AB6" s="8"/>
-      <c r="AC6" s="8"/>
-      <c r="AD6" s="8"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="8"/>
-      <c r="AG6" s="8"/>
-      <c r="AH6" s="8"/>
-      <c r="AI6" s="8"/>
-      <c r="AJ6" s="8"/>
-      <c r="AK6" s="9"/>
-      <c r="AN6" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AO6" s="4">
-        <v>16</v>
-      </c>
-      <c r="AP6" s="6">
-        <v>1</v>
-      </c>
-      <c r="AQ6" s="4">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AS6" s="4">
-        <f t="shared" si="1"/>
-        <v>65536</v>
-      </c>
-      <c r="AT6" s="4">
-        <v>0</v>
-      </c>
-    </row>
+      <c r="BC5" s="12"/>
+      <c r="BD5" s="12"/>
+      <c r="BE5" s="12"/>
+      <c r="BF5" s="12"/>
+      <c r="BG5" s="12"/>
+      <c r="BH5" s="12"/>
+      <c r="BI5" s="12"/>
+      <c r="BJ5" s="12"/>
+      <c r="BK5" s="12"/>
+      <c r="BL5" s="12"/>
+      <c r="BM5" s="12"/>
+      <c r="BN5" s="12"/>
+      <c r="BO5" s="12"/>
+      <c r="BP5" s="12"/>
+      <c r="BQ5" s="13"/>
+    </row>
+    <row r="6" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="27"/>
+      <c r="Y6" s="27"/>
+      <c r="Z6" s="27"/>
+      <c r="AA6" s="27"/>
+      <c r="AB6" s="27"/>
+      <c r="AC6" s="27"/>
+      <c r="AD6" s="28"/>
+      <c r="AE6" s="28"/>
+      <c r="AF6" s="28"/>
+      <c r="AG6" s="28"/>
+      <c r="AH6" s="28"/>
+      <c r="AI6" s="28"/>
+      <c r="AJ6" s="28"/>
+      <c r="AK6" s="28"/>
+      <c r="AL6" s="27"/>
+      <c r="AM6" s="27"/>
+      <c r="AN6" s="27"/>
+      <c r="AO6" s="27"/>
+      <c r="AP6" s="27"/>
+      <c r="AQ6" s="27"/>
+      <c r="AR6" s="27"/>
+      <c r="AS6" s="27"/>
+      <c r="AT6" s="26"/>
+      <c r="AU6" s="27"/>
+      <c r="AV6" s="27"/>
+      <c r="AW6" s="27"/>
+      <c r="AX6" s="26"/>
+      <c r="AY6" s="26"/>
+      <c r="AZ6" s="26"/>
+      <c r="BA6" s="26"/>
+      <c r="BB6" s="27"/>
+      <c r="BC6" s="27"/>
+      <c r="BD6" s="27"/>
+      <c r="BE6" s="27"/>
+      <c r="BF6" s="27"/>
+      <c r="BG6" s="27"/>
+      <c r="BH6" s="27"/>
+      <c r="BI6" s="27"/>
+      <c r="BJ6" s="28"/>
+      <c r="BK6" s="28"/>
+      <c r="BL6" s="28"/>
+      <c r="BM6" s="28"/>
+      <c r="BN6" s="28"/>
+      <c r="BO6" s="28"/>
+      <c r="BP6" s="28"/>
+      <c r="BQ6" s="28"/>
+    </row>
+    <row r="7" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="28"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="28"/>
+      <c r="AB7" s="28"/>
+      <c r="AC7" s="28"/>
+      <c r="AD7" s="28"/>
+      <c r="AE7" s="28"/>
+      <c r="AF7" s="28"/>
+      <c r="AG7" s="28"/>
+      <c r="AH7" s="28"/>
+      <c r="AI7" s="28"/>
+      <c r="AJ7" s="28"/>
+      <c r="AK7" s="28"/>
+      <c r="AL7" s="28"/>
+      <c r="AM7" s="28"/>
+      <c r="AN7" s="28"/>
+      <c r="AO7" s="28"/>
+      <c r="AP7" s="28"/>
+      <c r="AQ7" s="28"/>
+      <c r="AR7" s="28"/>
+      <c r="AS7" s="28"/>
+      <c r="AT7" s="28"/>
+      <c r="AU7" s="28"/>
+      <c r="AV7" s="28"/>
+      <c r="AW7" s="28"/>
+      <c r="AX7" s="28"/>
+      <c r="AY7" s="28"/>
+      <c r="AZ7" s="28"/>
+      <c r="BA7" s="28"/>
+      <c r="BB7" s="28"/>
+      <c r="BC7" s="28"/>
+      <c r="BD7" s="28"/>
+      <c r="BE7" s="28"/>
+      <c r="BF7" s="28"/>
+      <c r="BG7" s="28"/>
+      <c r="BH7" s="28"/>
+      <c r="BI7" s="28"/>
+      <c r="BJ7" s="28"/>
+      <c r="BK7" s="28"/>
+      <c r="BL7" s="28"/>
+      <c r="BM7" s="28"/>
+      <c r="BN7" s="28"/>
+      <c r="BO7" s="28"/>
+      <c r="BP7" s="28"/>
+      <c r="BQ7" s="28"/>
+    </row>
+    <row r="10" spans="1:69" ht="66.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:69" ht="69" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:69" ht="81.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:69" ht="93" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="37">
+    <mergeCell ref="BJ6:BM6"/>
+    <mergeCell ref="BN6:BQ6"/>
+    <mergeCell ref="AL7:BA7"/>
+    <mergeCell ref="BB7:BQ7"/>
+    <mergeCell ref="BB5:BQ5"/>
+    <mergeCell ref="AL2:AS2"/>
+    <mergeCell ref="AT2:BA2"/>
+    <mergeCell ref="BB2:BI2"/>
+    <mergeCell ref="BJ2:BQ2"/>
+    <mergeCell ref="AL4:BA4"/>
+    <mergeCell ref="BB4:BQ4"/>
+    <mergeCell ref="F7:U7"/>
+    <mergeCell ref="AD5:AG5"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="V4:AC4"/>
+    <mergeCell ref="F4:M4"/>
+    <mergeCell ref="N4:U4"/>
+    <mergeCell ref="V5:AC5"/>
+    <mergeCell ref="N5:U5"/>
     <mergeCell ref="F5:M5"/>
-    <mergeCell ref="N5:U5"/>
-    <mergeCell ref="F6:M6"/>
-    <mergeCell ref="N6:U6"/>
-    <mergeCell ref="F4:U4"/>
+    <mergeCell ref="AJ4:AK4"/>
+    <mergeCell ref="AH4:AI4"/>
+    <mergeCell ref="AH5:AI5"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="V2:AC2"/>
     <mergeCell ref="AD2:AK2"/>
@@ -2334,11 +2830,366 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="N2:U2"/>
-    <mergeCell ref="V4:AK4"/>
-    <mergeCell ref="V5:AK5"/>
-    <mergeCell ref="V6:AK6"/>
+    <mergeCell ref="AD6:AG6"/>
+    <mergeCell ref="AH6:AK6"/>
+    <mergeCell ref="V7:AK7"/>
+    <mergeCell ref="AL5:BA5"/>
+    <mergeCell ref="AJ5:AK5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="6">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="44"/>
+    </row>
+    <row r="5" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="6">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="6">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="6">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="6">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="6">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="6">
+        <v>4</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10" s="6">
+        <v>4</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added latest CAN Protocol
</commit_message>
<xml_diff>
--- a/1_Planning/System_Interface_Design.xlsx
+++ b/1_Planning/System_Interface_Design.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12885" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Signal List" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="128">
   <si>
     <t>System Interface Design</t>
   </si>
@@ -373,9 +373,6 @@
  its current error (if any) </t>
   </si>
   <si>
-    <t>*debug (empty)*</t>
-  </si>
-  <si>
     <t>0 to 65536</t>
   </si>
   <si>
@@ -423,13 +420,25 @@
   <si>
     <t>MC signal that commands PC to
  change X-axis paddle position in mm</t>
+  </si>
+  <si>
+    <t>*(empty)*</t>
+  </si>
+  <si>
+    <t>pc_status_debug</t>
+  </si>
+  <si>
+    <t>mc_cmd_pc_debug</t>
+  </si>
+  <si>
+    <t>NOTE: If you edit Messages/Signals here, make sure the changes match Enums in settings.JSON file \capstone\6_User_Interface\1_Software\4_Json\settings.json</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,8 +475,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,6 +528,16 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -611,13 +659,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -627,117 +678,125 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
     <cellStyle name="40% - Accent3" xfId="3" builtinId="39"/>
+    <cellStyle name="Bad" xfId="5" builtinId="27"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Warning Text" xfId="6" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1017,7 +1076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D198"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -2141,8 +2200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BQ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2163,337 +2222,337 @@
       </c>
     </row>
     <row r="2" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="35" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="36" t="s">
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="38"/>
-      <c r="AD2" s="35" t="s">
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="35"/>
-      <c r="AH2" s="35"/>
-      <c r="AI2" s="35"/>
-      <c r="AJ2" s="35"/>
-      <c r="AK2" s="35"/>
-      <c r="AL2" s="34" t="s">
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="19"/>
+      <c r="AH2" s="19"/>
+      <c r="AI2" s="19"/>
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
+      <c r="AL2" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="AM2" s="34"/>
-      <c r="AN2" s="34"/>
-      <c r="AO2" s="34"/>
-      <c r="AP2" s="34"/>
-      <c r="AQ2" s="34"/>
-      <c r="AR2" s="34"/>
-      <c r="AS2" s="34"/>
-      <c r="AT2" s="35" t="s">
+      <c r="AM2" s="18"/>
+      <c r="AN2" s="18"/>
+      <c r="AO2" s="18"/>
+      <c r="AP2" s="18"/>
+      <c r="AQ2" s="18"/>
+      <c r="AR2" s="18"/>
+      <c r="AS2" s="18"/>
+      <c r="AT2" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AU2" s="35"/>
-      <c r="AV2" s="35"/>
-      <c r="AW2" s="35"/>
-      <c r="AX2" s="35"/>
-      <c r="AY2" s="35"/>
-      <c r="AZ2" s="35"/>
-      <c r="BA2" s="35"/>
-      <c r="BB2" s="34" t="s">
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="19"/>
+      <c r="BB2" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="BC2" s="34"/>
-      <c r="BD2" s="34"/>
-      <c r="BE2" s="34"/>
-      <c r="BF2" s="34"/>
-      <c r="BG2" s="34"/>
-      <c r="BH2" s="34"/>
-      <c r="BI2" s="34"/>
-      <c r="BJ2" s="35" t="s">
+      <c r="BC2" s="18"/>
+      <c r="BD2" s="18"/>
+      <c r="BE2" s="18"/>
+      <c r="BF2" s="18"/>
+      <c r="BG2" s="18"/>
+      <c r="BH2" s="18"/>
+      <c r="BI2" s="18"/>
+      <c r="BJ2" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="BK2" s="35"/>
-      <c r="BL2" s="35"/>
-      <c r="BM2" s="35"/>
-      <c r="BN2" s="35"/>
-      <c r="BO2" s="35"/>
-      <c r="BP2" s="35"/>
-      <c r="BQ2" s="35"/>
+      <c r="BK2" s="19"/>
+      <c r="BL2" s="19"/>
+      <c r="BM2" s="19"/>
+      <c r="BN2" s="19"/>
+      <c r="BO2" s="19"/>
+      <c r="BP2" s="19"/>
+      <c r="BQ2" s="19"/>
     </row>
     <row r="3" spans="1:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="30">
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="11">
         <v>7</v>
       </c>
-      <c r="G3" s="30">
+      <c r="G3" s="11">
         <v>6</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="11">
         <v>5</v>
       </c>
-      <c r="I3" s="30">
+      <c r="I3" s="11">
         <v>4</v>
       </c>
-      <c r="J3" s="30">
+      <c r="J3" s="11">
         <v>3</v>
       </c>
-      <c r="K3" s="30">
+      <c r="K3" s="11">
         <v>2</v>
       </c>
-      <c r="L3" s="30">
+      <c r="L3" s="11">
         <v>1</v>
       </c>
-      <c r="M3" s="30">
+      <c r="M3" s="11">
         <v>0</v>
       </c>
-      <c r="N3" s="29">
+      <c r="N3" s="10">
         <v>7</v>
       </c>
-      <c r="O3" s="29">
+      <c r="O3" s="10">
         <v>6</v>
       </c>
-      <c r="P3" s="29">
+      <c r="P3" s="10">
         <v>5</v>
       </c>
-      <c r="Q3" s="29">
+      <c r="Q3" s="10">
         <v>4</v>
       </c>
-      <c r="R3" s="29">
+      <c r="R3" s="10">
         <v>3</v>
       </c>
-      <c r="S3" s="29">
+      <c r="S3" s="10">
         <v>2</v>
       </c>
-      <c r="T3" s="29">
+      <c r="T3" s="10">
         <v>1</v>
       </c>
-      <c r="U3" s="29">
+      <c r="U3" s="10">
         <v>0</v>
       </c>
-      <c r="V3" s="30">
+      <c r="V3" s="11">
         <v>7</v>
       </c>
-      <c r="W3" s="30">
+      <c r="W3" s="11">
         <v>6</v>
       </c>
-      <c r="X3" s="30">
+      <c r="X3" s="11">
         <v>5</v>
       </c>
-      <c r="Y3" s="30">
+      <c r="Y3" s="11">
         <v>4</v>
       </c>
-      <c r="Z3" s="30">
+      <c r="Z3" s="11">
         <v>3</v>
       </c>
-      <c r="AA3" s="30">
+      <c r="AA3" s="11">
         <v>2</v>
       </c>
-      <c r="AB3" s="30">
+      <c r="AB3" s="11">
         <v>1</v>
       </c>
-      <c r="AC3" s="30">
+      <c r="AC3" s="11">
         <v>0</v>
       </c>
-      <c r="AD3" s="29">
+      <c r="AD3" s="10">
         <v>7</v>
       </c>
-      <c r="AE3" s="29">
+      <c r="AE3" s="10">
         <v>6</v>
       </c>
-      <c r="AF3" s="29">
+      <c r="AF3" s="10">
         <v>5</v>
       </c>
-      <c r="AG3" s="29">
+      <c r="AG3" s="10">
         <v>4</v>
       </c>
-      <c r="AH3" s="29">
+      <c r="AH3" s="10">
         <v>3</v>
       </c>
-      <c r="AI3" s="29">
+      <c r="AI3" s="10">
         <v>2</v>
       </c>
-      <c r="AJ3" s="29">
+      <c r="AJ3" s="10">
         <v>1</v>
       </c>
-      <c r="AK3" s="29">
+      <c r="AK3" s="10">
         <v>0</v>
       </c>
-      <c r="AL3" s="30">
+      <c r="AL3" s="11">
         <v>7</v>
       </c>
-      <c r="AM3" s="30">
+      <c r="AM3" s="11">
         <v>6</v>
       </c>
-      <c r="AN3" s="30">
+      <c r="AN3" s="11">
         <v>5</v>
       </c>
-      <c r="AO3" s="30">
+      <c r="AO3" s="11">
         <v>4</v>
       </c>
-      <c r="AP3" s="30">
+      <c r="AP3" s="11">
         <v>3</v>
       </c>
-      <c r="AQ3" s="30">
+      <c r="AQ3" s="11">
         <v>2</v>
       </c>
-      <c r="AR3" s="30">
+      <c r="AR3" s="11">
         <v>1</v>
       </c>
-      <c r="AS3" s="30">
+      <c r="AS3" s="11">
         <v>0</v>
       </c>
-      <c r="AT3" s="29">
+      <c r="AT3" s="10">
         <v>7</v>
       </c>
-      <c r="AU3" s="29">
+      <c r="AU3" s="10">
         <v>6</v>
       </c>
-      <c r="AV3" s="29">
+      <c r="AV3" s="10">
         <v>5</v>
       </c>
-      <c r="AW3" s="29">
+      <c r="AW3" s="10">
         <v>4</v>
       </c>
-      <c r="AX3" s="29">
+      <c r="AX3" s="10">
         <v>3</v>
       </c>
-      <c r="AY3" s="29">
+      <c r="AY3" s="10">
         <v>2</v>
       </c>
-      <c r="AZ3" s="29">
+      <c r="AZ3" s="10">
         <v>1</v>
       </c>
-      <c r="BA3" s="29">
+      <c r="BA3" s="10">
         <v>0</v>
       </c>
-      <c r="BB3" s="30">
+      <c r="BB3" s="11">
         <v>7</v>
       </c>
-      <c r="BC3" s="30">
+      <c r="BC3" s="11">
         <v>6</v>
       </c>
-      <c r="BD3" s="30">
+      <c r="BD3" s="11">
         <v>5</v>
       </c>
-      <c r="BE3" s="30">
+      <c r="BE3" s="11">
         <v>4</v>
       </c>
-      <c r="BF3" s="30">
+      <c r="BF3" s="11">
         <v>3</v>
       </c>
-      <c r="BG3" s="30">
+      <c r="BG3" s="11">
         <v>2</v>
       </c>
-      <c r="BH3" s="30">
+      <c r="BH3" s="11">
         <v>1</v>
       </c>
-      <c r="BI3" s="30">
+      <c r="BI3" s="11">
         <v>0</v>
       </c>
-      <c r="BJ3" s="29">
+      <c r="BJ3" s="10">
         <v>7</v>
       </c>
-      <c r="BK3" s="29">
+      <c r="BK3" s="10">
         <v>6</v>
       </c>
-      <c r="BL3" s="29">
+      <c r="BL3" s="10">
         <v>5</v>
       </c>
-      <c r="BM3" s="29">
+      <c r="BM3" s="10">
         <v>4</v>
       </c>
-      <c r="BN3" s="29">
+      <c r="BN3" s="10">
         <v>3</v>
       </c>
-      <c r="BO3" s="29">
+      <c r="BO3" s="10">
         <v>2</v>
       </c>
-      <c r="BP3" s="29">
+      <c r="BP3" s="10">
         <v>1</v>
       </c>
-      <c r="BQ3" s="29">
+      <c r="BQ3" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:69" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="7">
         <v>8</v>
       </c>
-      <c r="F4" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
+      <c r="F4" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
       <c r="V4" s="20" t="s">
         <v>101</v>
       </c>
@@ -2504,18 +2563,18 @@
       <c r="AA4" s="21"/>
       <c r="AB4" s="21"/>
       <c r="AC4" s="22"/>
-      <c r="AD4" s="40"/>
-      <c r="AE4" s="40"/>
-      <c r="AF4" s="40"/>
-      <c r="AG4" s="40"/>
-      <c r="AH4" s="23" t="s">
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="23"/>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="23"/>
+      <c r="AH4" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="AI4" s="24"/>
-      <c r="AJ4" s="25" t="s">
+      <c r="AI4" s="27"/>
+      <c r="AJ4" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="AK4" s="24"/>
+      <c r="AK4" s="27"/>
       <c r="AL4" s="20" t="s">
         <v>82</v>
       </c>
@@ -2557,11 +2616,11 @@
       <c r="A5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="49" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>78</v>
@@ -2569,228 +2628,234 @@
       <c r="E5" s="4">
         <v>8</v>
       </c>
-      <c r="F5" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="11" t="s">
+      <c r="F5" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="11" t="s">
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="12"/>
-      <c r="AC5" s="12"/>
-      <c r="AD5" s="12" t="s">
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="AE5" s="12"/>
-      <c r="AF5" s="12"/>
-      <c r="AG5" s="13"/>
-      <c r="AH5" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI5" s="17"/>
-      <c r="AJ5" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="AK5" s="17"/>
-      <c r="AL5" s="11" t="s">
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI5" s="30"/>
+      <c r="AJ5" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="AK5" s="30"/>
+      <c r="AL5" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="AM5" s="12"/>
-      <c r="AN5" s="12"/>
-      <c r="AO5" s="12"/>
-      <c r="AP5" s="12"/>
-      <c r="AQ5" s="12"/>
-      <c r="AR5" s="12"/>
-      <c r="AS5" s="12"/>
-      <c r="AT5" s="12"/>
-      <c r="AU5" s="12"/>
-      <c r="AV5" s="12"/>
-      <c r="AW5" s="12"/>
-      <c r="AX5" s="12"/>
-      <c r="AY5" s="12"/>
-      <c r="AZ5" s="12"/>
-      <c r="BA5" s="13"/>
-      <c r="BB5" s="11" t="s">
+      <c r="AM5" s="16"/>
+      <c r="AN5" s="16"/>
+      <c r="AO5" s="16"/>
+      <c r="AP5" s="16"/>
+      <c r="AQ5" s="16"/>
+      <c r="AR5" s="16"/>
+      <c r="AS5" s="16"/>
+      <c r="AT5" s="16"/>
+      <c r="AU5" s="16"/>
+      <c r="AV5" s="16"/>
+      <c r="AW5" s="16"/>
+      <c r="AX5" s="16"/>
+      <c r="AY5" s="16"/>
+      <c r="AZ5" s="16"/>
+      <c r="BA5" s="17"/>
+      <c r="BB5" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="BC5" s="12"/>
-      <c r="BD5" s="12"/>
-      <c r="BE5" s="12"/>
-      <c r="BF5" s="12"/>
-      <c r="BG5" s="12"/>
-      <c r="BH5" s="12"/>
-      <c r="BI5" s="12"/>
-      <c r="BJ5" s="12"/>
-      <c r="BK5" s="12"/>
-      <c r="BL5" s="12"/>
-      <c r="BM5" s="12"/>
-      <c r="BN5" s="12"/>
-      <c r="BO5" s="12"/>
-      <c r="BP5" s="12"/>
-      <c r="BQ5" s="13"/>
+      <c r="BC5" s="16"/>
+      <c r="BD5" s="16"/>
+      <c r="BE5" s="16"/>
+      <c r="BF5" s="16"/>
+      <c r="BG5" s="16"/>
+      <c r="BH5" s="16"/>
+      <c r="BI5" s="16"/>
+      <c r="BJ5" s="16"/>
+      <c r="BK5" s="16"/>
+      <c r="BL5" s="16"/>
+      <c r="BM5" s="16"/>
+      <c r="BN5" s="16"/>
+      <c r="BO5" s="16"/>
+      <c r="BP5" s="16"/>
+      <c r="BQ5" s="17"/>
     </row>
     <row r="6" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="26"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26"/>
-      <c r="U6" s="26"/>
-      <c r="V6" s="27"/>
-      <c r="W6" s="27"/>
-      <c r="X6" s="27"/>
-      <c r="Y6" s="27"/>
-      <c r="Z6" s="27"/>
-      <c r="AA6" s="27"/>
-      <c r="AB6" s="27"/>
-      <c r="AC6" s="27"/>
-      <c r="AD6" s="28"/>
-      <c r="AE6" s="28"/>
-      <c r="AF6" s="28"/>
-      <c r="AG6" s="28"/>
-      <c r="AH6" s="28"/>
-      <c r="AI6" s="28"/>
-      <c r="AJ6" s="28"/>
-      <c r="AK6" s="28"/>
-      <c r="AL6" s="27"/>
-      <c r="AM6" s="27"/>
-      <c r="AN6" s="27"/>
-      <c r="AO6" s="27"/>
-      <c r="AP6" s="27"/>
-      <c r="AQ6" s="27"/>
-      <c r="AR6" s="27"/>
-      <c r="AS6" s="27"/>
-      <c r="AT6" s="26"/>
-      <c r="AU6" s="27"/>
-      <c r="AV6" s="27"/>
-      <c r="AW6" s="27"/>
-      <c r="AX6" s="26"/>
-      <c r="AY6" s="26"/>
-      <c r="AZ6" s="26"/>
-      <c r="BA6" s="26"/>
-      <c r="BB6" s="27"/>
-      <c r="BC6" s="27"/>
-      <c r="BD6" s="27"/>
-      <c r="BE6" s="27"/>
-      <c r="BF6" s="27"/>
-      <c r="BG6" s="27"/>
-      <c r="BH6" s="27"/>
-      <c r="BI6" s="27"/>
-      <c r="BJ6" s="28"/>
-      <c r="BK6" s="28"/>
-      <c r="BL6" s="28"/>
-      <c r="BM6" s="28"/>
-      <c r="BN6" s="28"/>
-      <c r="BO6" s="28"/>
-      <c r="BP6" s="28"/>
-      <c r="BQ6" s="28"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="14"/>
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="14"/>
+      <c r="AH6" s="14"/>
+      <c r="AI6" s="14"/>
+      <c r="AJ6" s="14"/>
+      <c r="AK6" s="14"/>
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="9"/>
+      <c r="AN6" s="9"/>
+      <c r="AO6" s="9"/>
+      <c r="AP6" s="9"/>
+      <c r="AQ6" s="9"/>
+      <c r="AR6" s="9"/>
+      <c r="AS6" s="9"/>
+      <c r="AT6" s="8"/>
+      <c r="AU6" s="9"/>
+      <c r="AV6" s="9"/>
+      <c r="AW6" s="9"/>
+      <c r="AX6" s="8"/>
+      <c r="AY6" s="8"/>
+      <c r="AZ6" s="8"/>
+      <c r="BA6" s="8"/>
+      <c r="BB6" s="9"/>
+      <c r="BC6" s="9"/>
+      <c r="BD6" s="9"/>
+      <c r="BE6" s="9"/>
+      <c r="BF6" s="9"/>
+      <c r="BG6" s="9"/>
+      <c r="BH6" s="9"/>
+      <c r="BI6" s="9"/>
+      <c r="BJ6" s="14"/>
+      <c r="BK6" s="14"/>
+      <c r="BL6" s="14"/>
+      <c r="BM6" s="14"/>
+      <c r="BN6" s="14"/>
+      <c r="BO6" s="14"/>
+      <c r="BP6" s="14"/>
+      <c r="BQ6" s="14"/>
     </row>
     <row r="7" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="28"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="28"/>
-      <c r="V7" s="28"/>
-      <c r="W7" s="28"/>
-      <c r="X7" s="28"/>
-      <c r="Y7" s="28"/>
-      <c r="Z7" s="28"/>
-      <c r="AA7" s="28"/>
-      <c r="AB7" s="28"/>
-      <c r="AC7" s="28"/>
-      <c r="AD7" s="28"/>
-      <c r="AE7" s="28"/>
-      <c r="AF7" s="28"/>
-      <c r="AG7" s="28"/>
-      <c r="AH7" s="28"/>
-      <c r="AI7" s="28"/>
-      <c r="AJ7" s="28"/>
-      <c r="AK7" s="28"/>
-      <c r="AL7" s="28"/>
-      <c r="AM7" s="28"/>
-      <c r="AN7" s="28"/>
-      <c r="AO7" s="28"/>
-      <c r="AP7" s="28"/>
-      <c r="AQ7" s="28"/>
-      <c r="AR7" s="28"/>
-      <c r="AS7" s="28"/>
-      <c r="AT7" s="28"/>
-      <c r="AU7" s="28"/>
-      <c r="AV7" s="28"/>
-      <c r="AW7" s="28"/>
-      <c r="AX7" s="28"/>
-      <c r="AY7" s="28"/>
-      <c r="AZ7" s="28"/>
-      <c r="BA7" s="28"/>
-      <c r="BB7" s="28"/>
-      <c r="BC7" s="28"/>
-      <c r="BD7" s="28"/>
-      <c r="BE7" s="28"/>
-      <c r="BF7" s="28"/>
-      <c r="BG7" s="28"/>
-      <c r="BH7" s="28"/>
-      <c r="BI7" s="28"/>
-      <c r="BJ7" s="28"/>
-      <c r="BK7" s="28"/>
-      <c r="BL7" s="28"/>
-      <c r="BM7" s="28"/>
-      <c r="BN7" s="28"/>
-      <c r="BO7" s="28"/>
-      <c r="BP7" s="28"/>
-      <c r="BQ7" s="28"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="14"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="14"/>
+      <c r="AE7" s="14"/>
+      <c r="AF7" s="14"/>
+      <c r="AG7" s="14"/>
+      <c r="AH7" s="14"/>
+      <c r="AI7" s="14"/>
+      <c r="AJ7" s="14"/>
+      <c r="AK7" s="14"/>
+      <c r="AL7" s="14"/>
+      <c r="AM7" s="14"/>
+      <c r="AN7" s="14"/>
+      <c r="AO7" s="14"/>
+      <c r="AP7" s="14"/>
+      <c r="AQ7" s="14"/>
+      <c r="AR7" s="14"/>
+      <c r="AS7" s="14"/>
+      <c r="AT7" s="14"/>
+      <c r="AU7" s="14"/>
+      <c r="AV7" s="14"/>
+      <c r="AW7" s="14"/>
+      <c r="AX7" s="14"/>
+      <c r="AY7" s="14"/>
+      <c r="AZ7" s="14"/>
+      <c r="BA7" s="14"/>
+      <c r="BB7" s="14"/>
+      <c r="BC7" s="14"/>
+      <c r="BD7" s="14"/>
+      <c r="BE7" s="14"/>
+      <c r="BF7" s="14"/>
+      <c r="BG7" s="14"/>
+      <c r="BH7" s="14"/>
+      <c r="BI7" s="14"/>
+      <c r="BJ7" s="14"/>
+      <c r="BK7" s="14"/>
+      <c r="BL7" s="14"/>
+      <c r="BM7" s="14"/>
+      <c r="BN7" s="14"/>
+      <c r="BO7" s="14"/>
+      <c r="BP7" s="14"/>
+      <c r="BQ7" s="14"/>
+    </row>
+    <row r="8" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="G8" s="50" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" s="2"/>
     </row>
     <row r="10" spans="1:69" ht="66.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:69" ht="69" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2798,26 +2863,10 @@
     <row r="13" spans="1:69" ht="93" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="BJ6:BM6"/>
-    <mergeCell ref="BN6:BQ6"/>
-    <mergeCell ref="AL7:BA7"/>
-    <mergeCell ref="BB7:BQ7"/>
-    <mergeCell ref="BB5:BQ5"/>
-    <mergeCell ref="AL2:AS2"/>
-    <mergeCell ref="AT2:BA2"/>
-    <mergeCell ref="BB2:BI2"/>
-    <mergeCell ref="BJ2:BQ2"/>
-    <mergeCell ref="AL4:BA4"/>
-    <mergeCell ref="BB4:BQ4"/>
-    <mergeCell ref="F7:U7"/>
-    <mergeCell ref="AD5:AG5"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="V4:AC4"/>
-    <mergeCell ref="F4:M4"/>
-    <mergeCell ref="N4:U4"/>
-    <mergeCell ref="V5:AC5"/>
-    <mergeCell ref="N5:U5"/>
-    <mergeCell ref="F5:M5"/>
+    <mergeCell ref="AH6:AK6"/>
+    <mergeCell ref="V7:AK7"/>
+    <mergeCell ref="AL5:BA5"/>
+    <mergeCell ref="AJ5:AK5"/>
     <mergeCell ref="AJ4:AK4"/>
     <mergeCell ref="AH4:AI4"/>
     <mergeCell ref="AH5:AI5"/>
@@ -2830,11 +2879,27 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="N2:U2"/>
+    <mergeCell ref="F7:U7"/>
+    <mergeCell ref="AD5:AG5"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="V4:AC4"/>
+    <mergeCell ref="F4:M4"/>
+    <mergeCell ref="N4:U4"/>
+    <mergeCell ref="V5:AC5"/>
+    <mergeCell ref="N5:U5"/>
+    <mergeCell ref="F5:M5"/>
     <mergeCell ref="AD6:AG6"/>
-    <mergeCell ref="AH6:AK6"/>
-    <mergeCell ref="V7:AK7"/>
-    <mergeCell ref="AL5:BA5"/>
-    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AL2:AS2"/>
+    <mergeCell ref="AT2:BA2"/>
+    <mergeCell ref="BB2:BI2"/>
+    <mergeCell ref="BJ2:BQ2"/>
+    <mergeCell ref="AL4:BA4"/>
+    <mergeCell ref="BB4:BQ4"/>
+    <mergeCell ref="BJ6:BM6"/>
+    <mergeCell ref="BN6:BQ6"/>
+    <mergeCell ref="AL7:BA7"/>
+    <mergeCell ref="BB7:BQ7"/>
+    <mergeCell ref="BB5:BQ5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="65" orientation="landscape" r:id="rId1"/>
@@ -2843,10 +2908,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2855,11 +2920,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
+      <c r="A1" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -2868,17 +2933,17 @@
       <c r="B3" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="31" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="39"/>
     </row>
     <row r="4" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -2887,17 +2952,17 @@
       <c r="B4" s="6">
         <v>16</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="44"/>
+      <c r="C4" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="42"/>
     </row>
     <row r="5" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -2906,89 +2971,94 @@
       <c r="B5" s="6">
         <v>16</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
+      <c r="C5" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="13" t="s">
         <v>100</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="9"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="44"/>
     </row>
     <row r="7" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="13" t="s">
         <v>99</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="44"/>
     </row>
     <row r="8" spans="1:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="13" t="s">
         <v>101</v>
       </c>
       <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="7" t="s">
+      <c r="C8" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="44"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="50" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="F8:I8"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:I3"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="F5:I5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="F8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2996,10 +3066,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3012,11 +3082,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="42" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
+      <c r="A1" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -3025,17 +3095,17 @@
       <c r="B3" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="31" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="33"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="39"/>
     </row>
     <row r="4" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -3044,17 +3114,17 @@
       <c r="B4" s="6">
         <v>16</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
+      <c r="C4" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
     </row>
     <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -3063,120 +3133,120 @@
       <c r="B5" s="6">
         <v>16</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
+      <c r="C5" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
     </row>
     <row r="6" spans="1:9" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="13" t="s">
         <v>93</v>
       </c>
       <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="9"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="44"/>
     </row>
     <row r="7" spans="1:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="13" t="s">
         <v>94</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="44"/>
     </row>
     <row r="8" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="13" t="s">
         <v>89</v>
       </c>
       <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="7" t="s">
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="44"/>
     </row>
     <row r="9" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="13" t="s">
         <v>102</v>
       </c>
       <c r="B9" s="6">
         <v>4</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="7" t="s">
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="44"/>
     </row>
     <row r="10" spans="1:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="13" t="s">
         <v>103</v>
       </c>
       <c r="B10" s="6">
         <v>4</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="7" t="s">
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="9"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="44"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="50" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:I5"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="F9:I9"/>
     <mergeCell ref="C3:E3"/>
@@ -3189,6 +3259,11 @@
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="C8:E8"/>
     <mergeCell ref="F8:I8"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>